<commit_message>
Liste mit Referenzen generieren
git-svn-id: svn://localhost/DI-Extractor@24 38a3ecd8-5b25-7645-a312-2ec681589999
</commit_message>
<xml_diff>
--- a/eCH-0160_2_xIsadg/eCH-0160 zu xIsadg_v3.xlsx
+++ b/eCH-0160_2_xIsadg/eCH-0160 zu xIsadg_v3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5970" windowWidth="25260" windowHeight="6030" tabRatio="861" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="5970" windowWidth="25260" windowHeight="6030" tabRatio="861"/>
   </bookViews>
   <sheets>
     <sheet name="eCH-0160 zu xIsadg" sheetId="13" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="6">'eCH-0160 Ordnungssystem'!$A$1:$K$9</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="7">'eCH-0160 Ordnungssystemposition'!$A$1:$K$16</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'eCH-0160 Provenienz'!$A$1:$K$12</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'eCH-0160 zu xIsadg'!$A$1:$I$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'eCH-0160 zu xIsadg'!$A$1:$I$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'ISAD(G)'!$A$1:$D$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">xIsadg!$A$2:$G$33</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">Crosswalk!$1:$1</definedName>
@@ -327,7 +327,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0">
+    <comment ref="A10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -336,8 +336,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">   &lt;xsl:element name="title"&gt;
+          <t xml:space="preserve">   &lt;!-- 3.1.2 Titel --&gt;
+   &lt;xsl:element name="title"&gt;
     &lt;xsl:choose&gt;
+     &lt;xsl:when test="$fondtitle"&gt;
+      &lt;xsl:value-of select="$fondtitle"/&gt;
+     &lt;/xsl:when&gt;
      &lt;xsl:when test="arelda:provenienz/arelda:registratur/text()"&gt;
       &lt;xsl:value-of select="arelda:provenienz/arelda:registratur"/&gt;
      &lt;/xsl:when&gt;
@@ -345,11 +349,12 @@
       &lt;xsl:value-of select="arelda:ordnungssystem/arelda:name"/&gt;
      &lt;/xsl:otherwise&gt;
     &lt;/xsl:choose&gt;
-   &lt;/xsl:element&gt;</t>
+   &lt;/xsl:element&gt;
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0">
+    <comment ref="D10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -365,7 +370,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0">
+    <comment ref="E10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -380,7 +385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0">
+    <comment ref="F10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -395,7 +400,45 @@
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="0">
+    <comment ref="A11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">   &lt;!-- 3.3.1 Form und Inhalt --&gt;
+   &lt;xsl:if test="arelda:ablieferungsteile/text()"&gt;
+    &lt;xsl:element name="scopeContent"&gt;
+     &lt;xsl:element name="content"&gt;
+      &lt;xsl:value-of select="arelda:ablieferungsteile"/&gt;
+     &lt;/xsl:element&gt;
+    &lt;/xsl:element&gt;
+   &lt;/xsl:if&gt;
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">      &lt;xsl:if test="arelda:Inhalt"&gt;
+       &lt;xsl:element name="content"&gt;
+        &lt;xsl:value-of select="arelda:Inhalt/text()"/&gt;
+       &lt;/xsl:element&gt;
+      &lt;/xsl:if&gt;</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -425,7 +468,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0">
+    <comment ref="F13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -455,7 +498,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E15" authorId="0">
+    <comment ref="E14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -503,7 +546,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F15" authorId="0">
+    <comment ref="F14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -522,7 +565,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E17" authorId="0">
+    <comment ref="E16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -533,13 +576,15 @@
           </rPr>
           <t xml:space="preserve">    &lt;xsl:if test="arelda:umfang/text()"&gt;
      &lt;xsl:element name="extentMedium"&gt;
-      &lt;xsl:value-of select="arelda:umfang/text()"/&gt;
+      &lt;xsl:element name="medium"&gt;
+       &lt;xsl:value-of select="arelda:umfang/text()"/&gt;
+      &lt;/xsl:element&gt;
      &lt;/xsl:element&gt;
     &lt;/xsl:if&gt;</t>
         </r>
       </text>
     </comment>
-    <comment ref="A21" authorId="0">
+    <comment ref="A20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -575,7 +620,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E21" authorId="0">
+    <comment ref="E20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -603,7 +648,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F21" authorId="0">
+    <comment ref="F20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -631,7 +676,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D28" authorId="0">
+    <comment ref="D27" authorId="0">
       <text>
         <r>
           <rPr>
@@ -657,7 +702,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E28" authorId="0">
+    <comment ref="E27" authorId="0">
       <text>
         <r>
           <rPr>
@@ -683,7 +728,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F28" authorId="0">
+    <comment ref="F27" authorId="0">
       <text>
         <r>
           <rPr>
@@ -709,7 +754,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A34" authorId="0">
+    <comment ref="A33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -736,7 +781,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E34" authorId="0">
+    <comment ref="E33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -753,7 +798,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F34" authorId="0">
+    <comment ref="F33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -770,7 +815,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A38" authorId="0">
+    <comment ref="A37" authorId="0">
       <text>
         <r>
           <rPr>
@@ -792,7 +837,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="625">
   <si>
     <t xml:space="preserve">Systeme, die mit dem beschriebenen System Daten ausgetauscht haben und damit Subsysteme, Parallelsysteme oder übergeordnete Systeme sind. Hier werden die Bezeichnungen der Systeme und die Art der Verwandtschaft eingetragen. </t>
   </si>
@@ -3006,12 +3051,81 @@
   <si>
     <t>ISAD(G): Dokument</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>extern:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Bestand-Titel</t>
+    </r>
+  </si>
+  <si>
+    <t>//scopeContent/scope</t>
+  </si>
+  <si>
+    <t>//scopeContent/content</t>
+  </si>
+  <si>
+    <t>//physTech</t>
+  </si>
+  <si>
+    <t>//identity/title</t>
+  </si>
+  <si>
+    <t>//context/creator</t>
+  </si>
+  <si>
+    <t>//identity/descriptionLevel</t>
+  </si>
+  <si>
+    <t>//context/acqInfo</t>
+  </si>
+  <si>
+    <t>//context/adminBioHistory</t>
+  </si>
+  <si>
+    <t>//identity/referenceCode</t>
+  </si>
+  <si>
+    <t>//context/archivalHistory</t>
+  </si>
+  <si>
+    <t>//identity/dates/fromDate
+//identity/dates/toDate</t>
+  </si>
+  <si>
+    <t>//notes/note</t>
+  </si>
+  <si>
+    <t>//contentStructure/appraisalDestruction</t>
+  </si>
+  <si>
+    <t>//extentMedium/medium</t>
+  </si>
+  <si>
+    <t>//accessConditions/hasPrivacyProtection
+//accessConditions/openToThePublic
+//accessConditions/classification
+//accessConditions/otherAccessConditions
+//accessConditions/accessConditionsNotes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3122,13 +3236,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -3593,17 +3700,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -3845,34 +3941,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="dashDotDot">
-        <color indexed="64"/>
-      </left>
-      <right style="dashDotDot">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="dashDotDot">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -3903,17 +3971,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashDotDot">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -3974,6 +4031,56 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashDotDot">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDotDot">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashDotDot">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -3986,7 +4093,7 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="212">
+  <cellXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4183,9 +4290,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4201,18 +4305,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4220,9 +4318,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4237,16 +4332,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -4335,199 +4430,175 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4587,6 +4658,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4616,6 +4696,72 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4693,8 +4839,8 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFFFFFCC"/>
       <color rgb="FFFFFF99"/>
-      <color rgb="FFFFFFCC"/>
       <color rgb="FFCCFFCC"/>
     </mruColors>
   </colors>
@@ -4989,23 +5135,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I41" sqref="A1:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="128" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" style="128" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="128" customWidth="1"/>
-    <col min="4" max="5" width="30.140625" style="128" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" style="128" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.28515625" style="128" customWidth="1"/>
-    <col min="8" max="8" width="26" style="128" customWidth="1"/>
-    <col min="9" max="9" width="29.85546875" style="128" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="128"/>
+    <col min="1" max="1" width="26.28515625" style="121" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" style="121" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="121" customWidth="1"/>
+    <col min="4" max="5" width="30.140625" style="121" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" style="121" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.28515625" style="121" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" style="121" customWidth="1"/>
+    <col min="9" max="9" width="37.28515625" style="127" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="121"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="13.5" thickBot="1">
@@ -5031,89 +5177,89 @@
       <c r="H1" s="53" t="s">
         <v>271</v>
       </c>
-      <c r="I1" s="120" t="s">
+      <c r="I1" s="115" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="26.25" thickBot="1">
-      <c r="A2" s="198" t="s">
+    <row r="2" spans="1:12" ht="13.5" thickBot="1">
+      <c r="A2" s="186" t="s">
         <v>605</v>
       </c>
-      <c r="B2" s="199"/>
-      <c r="C2" s="200"/>
-      <c r="D2" s="122" t="s">
+      <c r="B2" s="187"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="117" t="s">
         <v>606</v>
       </c>
-      <c r="E2" s="122" t="s">
+      <c r="E2" s="117" t="s">
         <v>607</v>
       </c>
-      <c r="F2" s="123" t="s">
+      <c r="F2" s="118" t="s">
         <v>608</v>
       </c>
-      <c r="G2" s="121"/>
+      <c r="G2" s="116"/>
       <c r="H2" s="48" t="s">
         <v>361</v>
       </c>
-      <c r="I2" s="124" t="s">
-        <v>286</v>
-      </c>
-      <c r="J2" s="129"/>
+      <c r="I2" s="209" t="s">
+        <v>615</v>
+      </c>
+      <c r="J2" s="122"/>
     </row>
     <row r="3" spans="1:12" ht="26.25" thickBot="1">
-      <c r="A3" s="167"/>
+      <c r="A3" s="156"/>
       <c r="B3" s="59" t="s">
         <v>79</v>
       </c>
       <c r="C3" s="54"/>
-      <c r="D3" s="159"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="141"/>
-      <c r="G3" s="160"/>
+      <c r="D3" s="149"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="150"/>
       <c r="H3" s="48" t="s">
         <v>363</v>
       </c>
-      <c r="I3" s="119" t="s">
-        <v>293</v>
-      </c>
-      <c r="J3" s="129"/>
-    </row>
-    <row r="4" spans="1:12" s="131" customFormat="1" ht="13.5" thickBot="1">
+      <c r="I3" s="114" t="s">
+        <v>614</v>
+      </c>
+      <c r="J3" s="122"/>
+    </row>
+    <row r="4" spans="1:12" s="124" customFormat="1" ht="13.5" thickBot="1">
       <c r="A4" s="59" t="s">
         <v>152</v>
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="54"/>
-      <c r="D4" s="159"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
-      <c r="G4" s="160"/>
+      <c r="D4" s="149"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="133"/>
+      <c r="G4" s="150"/>
       <c r="H4" s="49" t="s">
         <v>366</v>
       </c>
-      <c r="I4" s="83" t="s">
-        <v>302</v>
-      </c>
-      <c r="J4" s="130"/>
-    </row>
-    <row r="5" spans="1:12" s="131" customFormat="1" ht="26.25" thickBot="1">
-      <c r="A5" s="168"/>
+      <c r="I4" s="79" t="s">
+        <v>616</v>
+      </c>
+      <c r="J4" s="123"/>
+    </row>
+    <row r="5" spans="1:12" s="124" customFormat="1" ht="26.25" thickBot="1">
+      <c r="A5" s="157"/>
       <c r="B5" s="59" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="54"/>
-      <c r="D5" s="159"/>
-      <c r="E5" s="141"/>
-      <c r="F5" s="141"/>
-      <c r="G5" s="160"/>
+      <c r="D5" s="149"/>
+      <c r="E5" s="133"/>
+      <c r="F5" s="133"/>
+      <c r="G5" s="150"/>
       <c r="H5" s="49" t="s">
         <v>364</v>
       </c>
-      <c r="I5" s="83" t="s">
-        <v>296</v>
-      </c>
-      <c r="J5" s="130"/>
-    </row>
-    <row r="6" spans="1:12" ht="26.25" thickBot="1">
+      <c r="I5" s="79" t="s">
+        <v>617</v>
+      </c>
+      <c r="J5" s="123"/>
+    </row>
+    <row r="6" spans="1:12" ht="13.5" thickBot="1">
       <c r="A6" s="61" t="s">
         <v>111</v>
       </c>
@@ -5130,17 +5276,17 @@
         <v>132</v>
       </c>
       <c r="F6" s="62"/>
-      <c r="G6" s="160"/>
+      <c r="G6" s="150"/>
       <c r="H6" s="49" t="s">
         <v>358</v>
       </c>
-      <c r="I6" s="124" t="s">
-        <v>277</v>
-      </c>
-      <c r="J6" s="129"/>
-      <c r="L6" s="132"/>
-    </row>
-    <row r="7" spans="1:12" ht="26.25" thickBot="1">
+      <c r="I6" s="209" t="s">
+        <v>618</v>
+      </c>
+      <c r="J6" s="122"/>
+      <c r="L6" s="125"/>
+    </row>
+    <row r="7" spans="1:12" ht="13.5" thickBot="1">
       <c r="A7" s="56" t="s">
         <v>159</v>
       </c>
@@ -5148,621 +5294,608 @@
         <v>170</v>
       </c>
       <c r="C7" s="60"/>
-      <c r="D7" s="140"/>
+      <c r="D7" s="132"/>
       <c r="E7" s="56" t="s">
         <v>101</v>
       </c>
       <c r="F7" s="63"/>
-      <c r="G7" s="160"/>
+      <c r="G7" s="150"/>
       <c r="H7" s="49" t="s">
         <v>365</v>
       </c>
-      <c r="I7" s="173" t="s">
-        <v>299</v>
-      </c>
-      <c r="J7" s="129"/>
+      <c r="I7" s="79" t="s">
+        <v>619</v>
+      </c>
+      <c r="J7" s="122"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="158"/>
+      <c r="B8" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="57"/>
+      <c r="D8" s="148"/>
+      <c r="E8" s="135"/>
+      <c r="F8" s="135"/>
+      <c r="G8" s="152"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="78"/>
+    </row>
+    <row r="9" spans="1:12" ht="13.5" thickBot="1">
+      <c r="A9" s="77" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" s="70"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="147"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="153"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="78"/>
+    </row>
+    <row r="10" spans="1:12" ht="13.5" thickBot="1">
+      <c r="A10" s="190" t="s">
+        <v>609</v>
+      </c>
+      <c r="B10" s="191"/>
+      <c r="C10" s="192"/>
+      <c r="D10" s="72" t="s">
+        <v>133</v>
+      </c>
+      <c r="E10" s="72" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="72" t="s">
+        <v>133</v>
+      </c>
+      <c r="G10" s="64"/>
+      <c r="H10" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="I10" s="209" t="s">
+        <v>613</v>
+      </c>
+      <c r="J10" s="122"/>
+    </row>
+    <row r="11" spans="1:12" ht="13.5" thickBot="1">
+      <c r="A11" s="61" t="s">
         <v>129</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="158"/>
-      <c r="E8" s="142"/>
-      <c r="F8" s="143"/>
-      <c r="G8" s="161"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="125"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="169"/>
-      <c r="B9" s="70" t="s">
-        <v>176</v>
-      </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="157"/>
-      <c r="E9" s="144"/>
-      <c r="F9" s="144"/>
-      <c r="G9" s="162"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="82"/>
-    </row>
-    <row r="10" spans="1:12" ht="13.5" thickBot="1">
-      <c r="A10" s="70" t="s">
-        <v>151</v>
-      </c>
-      <c r="B10" s="71"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="156"/>
-      <c r="E10" s="145"/>
-      <c r="F10" s="163"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="82"/>
-    </row>
-    <row r="11" spans="1:12" ht="13.5" thickBot="1">
-      <c r="A11" s="153"/>
-      <c r="B11" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="C11" s="56" t="s">
-        <v>142</v>
-      </c>
-      <c r="D11" s="74" t="s">
-        <v>133</v>
-      </c>
-      <c r="E11" s="74" t="s">
-        <v>133</v>
-      </c>
-      <c r="F11" s="74" t="s">
-        <v>133</v>
-      </c>
-      <c r="G11" s="64"/>
-      <c r="H11" s="48" t="s">
-        <v>359</v>
-      </c>
-      <c r="I11" s="127" t="s">
-        <v>280</v>
-      </c>
-      <c r="J11" s="129"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="144"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="151"/>
-      <c r="E12" s="65" t="s">
+      <c r="B11" s="203"/>
+      <c r="C11" s="204"/>
+      <c r="D11" s="205"/>
+      <c r="E11" s="56" t="s">
         <v>180</v>
       </c>
-      <c r="F12" s="164"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="125"/>
-    </row>
-    <row r="13" spans="1:12" ht="13.5" thickBot="1">
-      <c r="A13" s="144"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="76" t="s">
+      <c r="F11" s="170"/>
+      <c r="G11" s="150"/>
+      <c r="H11" s="208" t="s">
+        <v>370</v>
+      </c>
+      <c r="I11" s="207" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="13.5" thickBot="1">
+      <c r="A12" s="134"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="167" t="s">
         <v>118</v>
       </c>
-      <c r="E13" s="55" t="s">
+      <c r="E12" s="206" t="s">
         <v>118</v>
       </c>
-      <c r="F13" s="55" t="s">
+      <c r="F12" s="206" t="s">
         <v>118</v>
       </c>
-      <c r="G13" s="58"/>
-      <c r="H13" s="69"/>
-      <c r="I13" s="82"/>
-    </row>
-    <row r="14" spans="1:12" ht="39" thickBot="1">
-      <c r="A14" s="144"/>
-      <c r="B14" s="67"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="153"/>
-      <c r="E14" s="74" t="s">
+      <c r="G12" s="58"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="78"/>
+    </row>
+    <row r="13" spans="1:12" ht="39" thickBot="1">
+      <c r="A13" s="135"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="F14" s="74" t="s">
+      <c r="F13" s="72" t="s">
         <v>105</v>
+      </c>
+      <c r="G13" s="64"/>
+      <c r="H13" s="48" t="s">
+        <v>378</v>
+      </c>
+      <c r="I13" s="79" t="s">
+        <v>612</v>
+      </c>
+      <c r="J13" s="122"/>
+    </row>
+    <row r="14" spans="1:12" ht="13.5" thickBot="1">
+      <c r="A14" s="135"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="143"/>
+      <c r="E14" s="56" t="s">
+        <v>183</v>
+      </c>
+      <c r="F14" s="56" t="s">
+        <v>20</v>
       </c>
       <c r="G14" s="64"/>
       <c r="H14" s="48" t="s">
-        <v>378</v>
-      </c>
-      <c r="I14" s="83" t="s">
-        <v>326</v>
-      </c>
-      <c r="J14" s="129"/>
-    </row>
-    <row r="15" spans="1:12" ht="39" thickBot="1">
-      <c r="A15" s="144"/>
-      <c r="B15" s="67"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="152"/>
-      <c r="E15" s="56" t="s">
-        <v>183</v>
-      </c>
-      <c r="F15" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="64"/>
-      <c r="H15" s="48" t="s">
         <v>370</v>
       </c>
-      <c r="I15" s="118" t="s">
-        <v>305</v>
-      </c>
-      <c r="J15" s="129"/>
-    </row>
-    <row r="16" spans="1:12" ht="13.5" thickBot="1">
-      <c r="A16" s="144"/>
-      <c r="B16" s="67"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="155"/>
-      <c r="E16" s="140"/>
-      <c r="F16" s="77" t="s">
+      <c r="I14" s="161" t="s">
+        <v>610</v>
+      </c>
+      <c r="J14" s="122"/>
+    </row>
+    <row r="15" spans="1:12" ht="13.5" thickBot="1">
+      <c r="A15" s="135"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="146"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="58"/>
-      <c r="H16" s="69"/>
-      <c r="I16" s="126"/>
-    </row>
-    <row r="17" spans="1:10" ht="39" thickBot="1">
-      <c r="A17" s="144"/>
-      <c r="B17" s="67"/>
-      <c r="C17" s="67"/>
-      <c r="D17" s="154"/>
-      <c r="E17" s="59" t="s">
+      <c r="G15" s="58"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="120"/>
+    </row>
+    <row r="16" spans="1:12" ht="26.25" thickBot="1">
+      <c r="A16" s="135"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="145"/>
+      <c r="E16" s="59" t="s">
         <v>175</v>
       </c>
-      <c r="F17" s="63"/>
-      <c r="G17" s="160"/>
-      <c r="H17" s="48" t="s">
+      <c r="F16" s="63"/>
+      <c r="G16" s="150"/>
+      <c r="H16" s="48" t="s">
         <v>362</v>
       </c>
-      <c r="I17" s="118" t="s">
-        <v>289</v>
-      </c>
-      <c r="J17" s="129"/>
-    </row>
-    <row r="18" spans="1:10" ht="25.5">
-      <c r="A18" s="144"/>
-      <c r="B18" s="67"/>
-      <c r="C18" s="67"/>
-      <c r="D18" s="76" t="s">
+      <c r="I16" s="161" t="s">
+        <v>623</v>
+      </c>
+      <c r="J16" s="122"/>
+    </row>
+    <row r="17" spans="1:10" s="213" customFormat="1">
+      <c r="A17" s="214"/>
+      <c r="B17" s="215"/>
+      <c r="C17" s="215"/>
+      <c r="D17" s="216" t="s">
         <v>102</v>
       </c>
-      <c r="E18" s="78" t="s">
+      <c r="E17" s="217" t="s">
         <v>102</v>
       </c>
-      <c r="F18" s="79" t="s">
+      <c r="F17" s="218" t="s">
         <v>116</v>
       </c>
+      <c r="G17" s="219"/>
+      <c r="H17" s="220"/>
+      <c r="I17" s="221"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="135"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="144"/>
+      <c r="E18" s="76" t="s">
+        <v>160</v>
+      </c>
+      <c r="F18" s="76" t="s">
+        <v>140</v>
+      </c>
       <c r="G18" s="58"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="125"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="144"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="153"/>
-      <c r="E19" s="80" t="s">
-        <v>160</v>
-      </c>
-      <c r="F19" s="80" t="s">
-        <v>140</v>
-      </c>
-      <c r="G19" s="58"/>
-      <c r="H19" s="69"/>
-      <c r="I19" s="82"/>
-    </row>
-    <row r="20" spans="1:10" ht="13.5" thickBot="1">
-      <c r="A20" s="170"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="152"/>
-      <c r="E20" s="81" t="s">
+      <c r="H18" s="68"/>
+      <c r="I18" s="78"/>
+    </row>
+    <row r="19" spans="1:10" ht="13.5" thickBot="1">
+      <c r="A19" s="136"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="143"/>
+      <c r="E19" s="77" t="s">
         <v>136</v>
       </c>
-      <c r="F20" s="67"/>
-      <c r="G20" s="165"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="82"/>
-    </row>
-    <row r="21" spans="1:10" ht="26.25" thickBot="1">
-      <c r="A21" s="76" t="s">
+      <c r="F19" s="66"/>
+      <c r="G19" s="154"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="78"/>
+    </row>
+    <row r="20" spans="1:10" ht="26.25" thickBot="1">
+      <c r="A20" s="206" t="s">
         <v>137</v>
       </c>
-      <c r="B21" s="80" t="s">
+      <c r="B20" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="C21" s="80" t="s">
+      <c r="C20" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="67"/>
-      <c r="E21" s="74" t="s">
+      <c r="D20" s="223"/>
+      <c r="E20" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="F21" s="74" t="s">
+      <c r="F20" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="G21" s="64"/>
-      <c r="H21" s="48" t="s">
+      <c r="G20" s="64"/>
+      <c r="H20" s="48" t="s">
         <v>360</v>
       </c>
-      <c r="I21" s="118" t="s">
-        <v>283</v>
-      </c>
-      <c r="J21" s="129"/>
+      <c r="I20" s="161" t="s">
+        <v>620</v>
+      </c>
+      <c r="J20" s="122"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="134"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="222"/>
+      <c r="D21" s="205"/>
+      <c r="E21" s="65" t="s">
+        <v>154</v>
+      </c>
+      <c r="F21" s="57"/>
+      <c r="G21" s="151"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="119"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="171"/>
-      <c r="B22" s="67"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="152"/>
-      <c r="E22" s="65" t="s">
-        <v>154</v>
-      </c>
-      <c r="F22" s="57"/>
-      <c r="G22" s="161"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="125"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="144"/>
-      <c r="B23" s="67"/>
-      <c r="C23" s="70" t="s">
+      <c r="A22" s="135"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="69" t="s">
         <v>144</v>
       </c>
-      <c r="D23" s="67"/>
-      <c r="E23" s="171"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="162"/>
-      <c r="H23" s="69"/>
-      <c r="I23" s="82"/>
-    </row>
-    <row r="24" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A24" s="70" t="s">
+      <c r="D22" s="66"/>
+      <c r="E22" s="159"/>
+      <c r="F22" s="135"/>
+      <c r="G22" s="152"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="78"/>
+    </row>
+    <row r="23" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A23" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="B24" s="174"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="176"/>
-      <c r="E24" s="176"/>
+      <c r="B23" s="162"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="164"/>
+      <c r="E23" s="164"/>
+      <c r="F23" s="146"/>
+      <c r="G23" s="152"/>
+      <c r="H23" s="125"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="73" t="s">
+        <v>165</v>
+      </c>
+      <c r="B24" s="66"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="73" t="s">
+        <v>165</v>
+      </c>
+      <c r="E24" s="73" t="s">
+        <v>165</v>
+      </c>
       <c r="F24" s="155"/>
-      <c r="G24" s="162"/>
-      <c r="H24" s="132"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="125"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="76" t="s">
-        <v>165</v>
-      </c>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="76" t="s">
-        <v>165</v>
-      </c>
-      <c r="E25" s="76" t="s">
-        <v>165</v>
-      </c>
-      <c r="F25" s="166"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="132"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="76" t="s">
+      <c r="A25" s="73" t="s">
         <v>162</v>
       </c>
-      <c r="B26" s="67"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="76" t="s">
+      <c r="B25" s="66"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="73" t="s">
         <v>162</v>
       </c>
-      <c r="E26" s="76" t="s">
+      <c r="E25" s="73" t="s">
         <v>162</v>
       </c>
-      <c r="F26" s="67"/>
-      <c r="G26" s="162"/>
-      <c r="H26" s="132"/>
-    </row>
-    <row r="27" spans="1:10" ht="13.5" thickBot="1">
-      <c r="A27" s="171"/>
-      <c r="B27" s="67"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="55" t="s">
+      <c r="F25" s="66"/>
+      <c r="G25" s="152"/>
+      <c r="H25" s="125"/>
+    </row>
+    <row r="26" spans="1:10" ht="13.5" thickBot="1">
+      <c r="A26" s="159"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="55" t="s">
         <v>150</v>
       </c>
-      <c r="E27" s="55" t="s">
+      <c r="E26" s="55" t="s">
         <v>150</v>
       </c>
-      <c r="F27" s="166"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="132"/>
-    </row>
-    <row r="28" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A28" s="144"/>
-      <c r="B28" s="67"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="179" t="s">
+      <c r="F26" s="155"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="125"/>
+    </row>
+    <row r="27" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A27" s="135"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="167" t="s">
         <v>134</v>
       </c>
-      <c r="E28" s="179" t="s">
+      <c r="E27" s="167" t="s">
         <v>134</v>
       </c>
-      <c r="F28" s="179" t="s">
+      <c r="F27" s="167" t="s">
         <v>134</v>
       </c>
-      <c r="G28" s="180"/>
-      <c r="H28" s="193" t="s">
+      <c r="G27" s="168"/>
+      <c r="H27" s="181" t="s">
         <v>375</v>
       </c>
-      <c r="I28" s="193" t="s">
-        <v>318</v>
-      </c>
+      <c r="I27" s="210" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="135"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="73" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="73" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="73" t="s">
+        <v>91</v>
+      </c>
+      <c r="G28" s="67"/>
+      <c r="H28" s="182"/>
+      <c r="I28" s="211"/>
+      <c r="J28" s="125"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="144"/>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="76" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" s="76" t="s">
-        <v>91</v>
-      </c>
-      <c r="F29" s="76" t="s">
-        <v>91</v>
-      </c>
-      <c r="G29" s="68"/>
-      <c r="H29" s="194"/>
-      <c r="I29" s="194"/>
-      <c r="J29" s="132"/>
+      <c r="A29" s="135"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="73" t="s">
+        <v>114</v>
+      </c>
+      <c r="E29" s="73" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="73" t="s">
+        <v>114</v>
+      </c>
+      <c r="G29" s="67"/>
+      <c r="H29" s="182"/>
+      <c r="I29" s="211"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="144"/>
-      <c r="B30" s="67"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="76" t="s">
-        <v>114</v>
-      </c>
-      <c r="E30" s="76" t="s">
-        <v>114</v>
-      </c>
-      <c r="F30" s="76" t="s">
-        <v>114</v>
-      </c>
-      <c r="G30" s="68"/>
-      <c r="H30" s="194"/>
-      <c r="I30" s="194"/>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="144"/>
-      <c r="B31" s="67"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="76" t="s">
+      <c r="A30" s="135"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="73" t="s">
         <v>161</v>
       </c>
-      <c r="E31" s="76" t="s">
+      <c r="E30" s="73" t="s">
         <v>161</v>
       </c>
-      <c r="F31" s="76" t="s">
+      <c r="F30" s="73" t="s">
         <v>161</v>
       </c>
-      <c r="G31" s="178"/>
-      <c r="H31" s="194"/>
-      <c r="I31" s="194"/>
+      <c r="G30" s="166"/>
+      <c r="H30" s="182"/>
+      <c r="I30" s="211"/>
+    </row>
+    <row r="31" spans="1:10" ht="13.5" thickBot="1">
+      <c r="A31" s="135"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="163"/>
+      <c r="D31" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="G31" s="58"/>
+      <c r="H31" s="183"/>
+      <c r="I31" s="212"/>
     </row>
     <row r="32" spans="1:10" ht="13.5" thickBot="1">
-      <c r="A32" s="144"/>
-      <c r="B32" s="67"/>
-      <c r="C32" s="175"/>
-      <c r="D32" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="E32" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="F32" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="G32" s="58"/>
-      <c r="H32" s="195"/>
-      <c r="I32" s="195"/>
-    </row>
-    <row r="33" spans="1:10" ht="13.5" thickBot="1">
-      <c r="A33" s="145"/>
-      <c r="B33" s="67"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="181"/>
-      <c r="E33" s="59" t="s">
+      <c r="A32" s="136"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="169"/>
+      <c r="E32" s="59" t="s">
         <v>158</v>
       </c>
-      <c r="F33" s="182"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="63"/>
-      <c r="I33" s="126"/>
-    </row>
-    <row r="34" spans="1:10" ht="26.25" thickBot="1">
-      <c r="A34" s="74" t="s">
+      <c r="F32" s="170"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="120"/>
+    </row>
+    <row r="33" spans="1:10" ht="26.25" thickBot="1">
+      <c r="A33" s="72" t="s">
         <v>135</v>
       </c>
-      <c r="B34" s="74" t="s">
+      <c r="B33" s="72" t="s">
         <v>135</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C33" s="72" t="s">
         <v>135</v>
       </c>
-      <c r="D34" s="63"/>
-      <c r="E34" s="177" t="s">
+      <c r="D33" s="63"/>
+      <c r="E33" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="F34" s="74" t="s">
+      <c r="F33" s="72" t="s">
         <v>135</v>
       </c>
-      <c r="G34" s="64"/>
-      <c r="H34" s="133" t="s">
+      <c r="G33" s="64"/>
+      <c r="H33" s="126" t="s">
         <v>386</v>
       </c>
-      <c r="I34" s="134" t="s">
-        <v>346</v>
-      </c>
-      <c r="J34" s="129"/>
+      <c r="I33" s="224" t="s">
+        <v>621</v>
+      </c>
+      <c r="J33" s="122"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="138"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="142"/>
+      <c r="E34" s="75" t="s">
+        <v>156</v>
+      </c>
+      <c r="F34" s="75" t="s">
+        <v>156</v>
+      </c>
+      <c r="G34" s="58"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="119"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="147"/>
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="151"/>
-      <c r="E35" s="78" t="s">
-        <v>156</v>
-      </c>
-      <c r="F35" s="78" t="s">
-        <v>156</v>
+      <c r="A35" s="73" t="s">
+        <v>260</v>
+      </c>
+      <c r="B35" s="66"/>
+      <c r="C35" s="73" t="s">
+        <v>260</v>
+      </c>
+      <c r="D35" s="73" t="s">
+        <v>260</v>
+      </c>
+      <c r="E35" s="73" t="s">
+        <v>260</v>
+      </c>
+      <c r="F35" s="73" t="s">
+        <v>260</v>
       </c>
       <c r="G35" s="58"/>
-      <c r="H35" s="69"/>
-      <c r="I35" s="125"/>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="76" t="s">
-        <v>260</v>
-      </c>
-      <c r="B36" s="67"/>
-      <c r="C36" s="76" t="s">
-        <v>260</v>
-      </c>
-      <c r="D36" s="76" t="s">
-        <v>260</v>
-      </c>
-      <c r="E36" s="76" t="s">
-        <v>260</v>
-      </c>
-      <c r="F36" s="76" t="s">
-        <v>260</v>
-      </c>
-      <c r="G36" s="58"/>
-      <c r="H36" s="69"/>
-      <c r="I36" s="82"/>
-    </row>
-    <row r="37" spans="1:10" ht="13.5" thickBot="1">
-      <c r="A37" s="172"/>
-      <c r="B37" s="81" t="s">
+      <c r="H35" s="68"/>
+      <c r="I35" s="78"/>
+    </row>
+    <row r="36" spans="1:10" ht="13.5" thickBot="1">
+      <c r="A36" s="160"/>
+      <c r="B36" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="67"/>
-      <c r="D37" s="150"/>
-      <c r="E37" s="146"/>
-      <c r="F37" s="146"/>
-      <c r="G37" s="165"/>
-      <c r="H37" s="69"/>
-      <c r="I37" s="82"/>
-    </row>
-    <row r="38" spans="1:10" ht="26.25" thickBot="1">
-      <c r="A38" s="59" t="s">
+      <c r="C36" s="66"/>
+      <c r="D36" s="141"/>
+      <c r="E36" s="137"/>
+      <c r="F36" s="137"/>
+      <c r="G36" s="154"/>
+      <c r="H36" s="68"/>
+      <c r="I36" s="78"/>
+    </row>
+    <row r="37" spans="1:10" ht="26.25" thickBot="1">
+      <c r="A37" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="63"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="149"/>
-      <c r="E38" s="148"/>
-      <c r="F38" s="148"/>
-      <c r="G38" s="160"/>
-      <c r="H38" s="48" t="s">
+      <c r="B37" s="63"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="140"/>
+      <c r="E37" s="139"/>
+      <c r="F37" s="139"/>
+      <c r="G37" s="150"/>
+      <c r="H37" s="48" t="s">
         <v>371</v>
       </c>
-      <c r="I38" s="173" t="s">
-        <v>308</v>
-      </c>
-      <c r="J38" s="129"/>
-    </row>
-    <row r="39" spans="1:10" ht="31.5" customHeight="1">
-      <c r="A39" s="135"/>
-      <c r="B39" s="135"/>
-      <c r="C39" s="135"/>
-      <c r="D39" s="135"/>
-      <c r="E39" s="135"/>
-      <c r="F39" s="135"/>
-      <c r="G39" s="135"/>
-      <c r="H39" s="135"/>
-      <c r="I39" s="136"/>
+      <c r="I37" s="161" t="s">
+        <v>622</v>
+      </c>
+      <c r="J37" s="122"/>
+    </row>
+    <row r="38" spans="1:10" ht="31.5" customHeight="1">
+      <c r="A38" s="127"/>
+      <c r="B38" s="127"/>
+      <c r="C38" s="127"/>
+      <c r="D38" s="127"/>
+      <c r="E38" s="127"/>
+      <c r="F38" s="127"/>
+      <c r="G38" s="127"/>
+      <c r="H38" s="127"/>
+      <c r="I38" s="128"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="189" t="s">
+        <v>391</v>
+      </c>
+      <c r="B39" s="189"/>
+      <c r="C39" s="129"/>
+      <c r="D39" s="127"/>
+      <c r="E39" s="127"/>
+      <c r="F39" s="127"/>
+      <c r="G39" s="127"/>
+      <c r="H39" s="127"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="201" t="s">
-        <v>391</v>
-      </c>
-      <c r="B40" s="201"/>
-      <c r="C40" s="137"/>
-      <c r="D40" s="135"/>
-      <c r="E40" s="135"/>
-      <c r="F40" s="135"/>
-      <c r="G40" s="135"/>
-      <c r="H40" s="135"/>
-      <c r="I40" s="135"/>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="201" t="s">
+      <c r="A40" s="189" t="s">
         <v>392</v>
       </c>
-      <c r="B41" s="201"/>
-      <c r="C41" s="138"/>
-      <c r="D41" s="135"/>
-      <c r="E41" s="135"/>
-      <c r="F41" s="135"/>
-      <c r="G41" s="135"/>
-      <c r="H41" s="135"/>
-      <c r="I41" s="135"/>
-      <c r="J41" s="132"/>
-    </row>
-    <row r="42" spans="1:10" ht="26.25" customHeight="1">
-      <c r="A42" s="196" t="s">
+      <c r="B40" s="189"/>
+      <c r="C40" s="130"/>
+      <c r="D40" s="127"/>
+      <c r="E40" s="127"/>
+      <c r="F40" s="127"/>
+      <c r="G40" s="127"/>
+      <c r="H40" s="127"/>
+      <c r="J40" s="125"/>
+    </row>
+    <row r="41" spans="1:10" ht="26.25" customHeight="1">
+      <c r="A41" s="184" t="s">
         <v>393</v>
       </c>
-      <c r="B42" s="197"/>
-      <c r="C42" s="139"/>
-      <c r="D42" s="135"/>
-      <c r="E42" s="135"/>
-      <c r="F42" s="135"/>
-      <c r="G42" s="135"/>
-      <c r="H42" s="135"/>
-      <c r="I42" s="135"/>
-      <c r="J42" s="132"/>
+      <c r="B41" s="185"/>
+      <c r="C41" s="131"/>
+      <c r="D41" s="127"/>
+      <c r="E41" s="127"/>
+      <c r="F41" s="127"/>
+      <c r="G41" s="127"/>
+      <c r="H41" s="127"/>
+      <c r="J41" s="125"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="127"/>
+      <c r="B42" s="127"/>
+      <c r="C42" s="127"/>
+      <c r="D42" s="127"/>
+      <c r="E42" s="127"/>
+      <c r="F42" s="127"/>
+      <c r="G42" s="127"/>
+      <c r="H42" s="127"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="135"/>
-      <c r="B43" s="135"/>
-      <c r="C43" s="135"/>
-      <c r="D43" s="135"/>
-      <c r="E43" s="135"/>
-      <c r="F43" s="135"/>
-      <c r="G43" s="135"/>
-      <c r="H43" s="135"/>
-      <c r="I43" s="135"/>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="135"/>
-      <c r="B44" s="135"/>
-      <c r="C44" s="135"/>
-      <c r="D44" s="135"/>
-      <c r="E44" s="135"/>
-      <c r="F44" s="135"/>
-      <c r="G44" s="135"/>
-      <c r="H44" s="135"/>
-      <c r="I44" s="135"/>
+      <c r="A43" s="127"/>
+      <c r="B43" s="127"/>
+      <c r="C43" s="127"/>
+      <c r="D43" s="127"/>
+      <c r="E43" s="127"/>
+      <c r="F43" s="127"/>
+      <c r="G43" s="127"/>
+      <c r="H43" s="127"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="H28:H32"/>
-    <mergeCell ref="I28:I32"/>
-    <mergeCell ref="A42:B42"/>
+  <mergeCells count="7">
+    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A39:B39"/>
     <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A10:C10"/>
   </mergeCells>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="61" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Arial,Fett"&amp;12&amp;A</oddHeader>
@@ -5802,10 +5935,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" customHeight="1">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="200" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="210"/>
+      <c r="B1" s="201"/>
     </row>
     <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5">
       <c r="A3" s="32" t="s">
@@ -6363,8 +6496,8 @@
   </sheetPr>
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -6376,26 +6509,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="202" t="s">
+      <c r="A1" s="193" t="s">
         <v>271</v>
       </c>
-      <c r="B1" s="203"/>
-      <c r="C1" s="187" t="s">
+      <c r="B1" s="194"/>
+      <c r="C1" s="175" t="s">
         <v>273</v>
       </c>
-      <c r="D1" s="188" t="s">
+      <c r="D1" s="176" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="25.5">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="171" t="s">
         <v>274</v>
       </c>
-      <c r="B2" s="184" t="s">
+      <c r="B2" s="172" t="s">
         <v>367</v>
       </c>
-      <c r="C2" s="185"/>
-      <c r="D2" s="186"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="174"/>
     </row>
     <row r="3" spans="1:4" ht="102">
       <c r="A3" s="39" t="s">
@@ -6468,14 +6601,14 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="183" t="s">
+      <c r="A8" s="171" t="s">
         <v>290</v>
       </c>
-      <c r="B8" s="184" t="s">
+      <c r="B8" s="172" t="s">
         <v>368</v>
       </c>
-      <c r="C8" s="185"/>
-      <c r="D8" s="186"/>
+      <c r="C8" s="173"/>
+      <c r="D8" s="174"/>
     </row>
     <row r="9" spans="1:4" ht="25.5">
       <c r="A9" s="39" t="s">
@@ -6534,23 +6667,23 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5">
-      <c r="A13" s="183" t="s">
+      <c r="A13" s="171" t="s">
         <v>303</v>
       </c>
-      <c r="B13" s="184" t="s">
+      <c r="B13" s="172" t="s">
         <v>369</v>
       </c>
-      <c r="C13" s="185"/>
-      <c r="D13" s="186"/>
+      <c r="C13" s="173"/>
+      <c r="D13" s="174"/>
     </row>
     <row r="14" spans="1:4" ht="89.25">
       <c r="A14" s="39" t="s">
         <v>304</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="47" t="s">
         <v>370</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="47" t="s">
         <v>305</v>
       </c>
       <c r="D14" s="40" t="s">
@@ -6600,14 +6733,14 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.5">
-      <c r="A18" s="183" t="s">
+      <c r="A18" s="171" t="s">
         <v>315</v>
       </c>
-      <c r="B18" s="184" t="s">
+      <c r="B18" s="172" t="s">
         <v>374</v>
       </c>
-      <c r="C18" s="185"/>
-      <c r="D18" s="186"/>
+      <c r="C18" s="173"/>
+      <c r="D18" s="174"/>
     </row>
     <row r="19" spans="1:4" ht="76.5">
       <c r="A19" s="39" t="s">
@@ -6680,14 +6813,14 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="183" t="s">
+      <c r="A24" s="171" t="s">
         <v>330</v>
       </c>
-      <c r="B24" s="184" t="s">
+      <c r="B24" s="172" t="s">
         <v>380</v>
       </c>
-      <c r="C24" s="185"/>
-      <c r="D24" s="186"/>
+      <c r="C24" s="173"/>
+      <c r="D24" s="174"/>
     </row>
     <row r="25" spans="1:4" ht="25.5">
       <c r="A25" s="41" t="s">
@@ -6704,16 +6837,16 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="25.5">
-      <c r="A26" s="189" t="s">
+      <c r="A26" s="177" t="s">
         <v>334</v>
       </c>
-      <c r="B26" s="190" t="s">
+      <c r="B26" s="178" t="s">
         <v>382</v>
       </c>
-      <c r="C26" s="190" t="s">
+      <c r="C26" s="178" t="s">
         <v>336</v>
       </c>
-      <c r="D26" s="191" t="s">
+      <c r="D26" s="179" t="s">
         <v>335</v>
       </c>
     </row>
@@ -6746,14 +6879,14 @@
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="183" t="s">
+      <c r="A29" s="171" t="s">
         <v>343</v>
       </c>
-      <c r="B29" s="184" t="s">
+      <c r="B29" s="172" t="s">
         <v>385</v>
       </c>
-      <c r="C29" s="185"/>
-      <c r="D29" s="186"/>
+      <c r="C29" s="173"/>
+      <c r="D29" s="174"/>
     </row>
     <row r="30" spans="1:4" ht="25.5">
       <c r="A30" s="39" t="s">
@@ -6770,14 +6903,14 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="25.5">
-      <c r="A31" s="183" t="s">
+      <c r="A31" s="171" t="s">
         <v>347</v>
       </c>
-      <c r="B31" s="184" t="s">
+      <c r="B31" s="172" t="s">
         <v>387</v>
       </c>
-      <c r="C31" s="185"/>
-      <c r="D31" s="186"/>
+      <c r="C31" s="173"/>
+      <c r="D31" s="174"/>
     </row>
     <row r="32" spans="1:4" ht="63.75">
       <c r="A32" s="41" t="s">
@@ -6822,20 +6955,20 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="204" t="s">
+      <c r="A36" s="195" t="s">
         <v>394</v>
       </c>
-      <c r="B36" s="204"/>
+      <c r="B36" s="195"/>
       <c r="C36" s="42" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="204" t="s">
+      <c r="A37" s="195" t="s">
         <v>395</v>
       </c>
-      <c r="B37" s="204"/>
-      <c r="C37" s="192" t="s">
+      <c r="B37" s="195"/>
+      <c r="C37" s="180" t="s">
         <v>396</v>
       </c>
     </row>
@@ -6864,772 +6997,772 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="88" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" style="88" customWidth="1"/>
-    <col min="3" max="3" width="73.5703125" style="88" customWidth="1"/>
-    <col min="4" max="4" width="37" style="88" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" style="88" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="88" customWidth="1"/>
-    <col min="7" max="7" width="119.7109375" style="88" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="88"/>
+    <col min="1" max="1" width="25.28515625" style="84" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" style="84" customWidth="1"/>
+    <col min="3" max="3" width="73.5703125" style="84" customWidth="1"/>
+    <col min="4" max="4" width="37" style="84" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" style="84" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="84" customWidth="1"/>
+    <col min="7" max="7" width="119.7109375" style="84" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="84"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.5" thickBot="1">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="80" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="86" t="s">
+      <c r="C1" s="82" t="s">
         <v>397</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="82" t="s">
         <v>398</v>
       </c>
-      <c r="E1" s="86" t="s">
+      <c r="E1" s="82" t="s">
         <v>399</v>
       </c>
-      <c r="F1" s="86" t="s">
+      <c r="F1" s="82" t="s">
         <v>400</v>
       </c>
-      <c r="G1" s="87" t="s">
+      <c r="G1" s="83" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="25.5">
-      <c r="A2" s="89">
+      <c r="A2" s="85">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="86" t="s">
         <v>402</v>
       </c>
-      <c r="C2" s="91" t="s">
+      <c r="C2" s="87" t="s">
         <v>403</v>
       </c>
-      <c r="D2" s="91" t="s">
+      <c r="D2" s="87" t="s">
         <v>404</v>
       </c>
-      <c r="E2" s="91" t="s">
+      <c r="E2" s="87" t="s">
         <v>405</v>
       </c>
-      <c r="F2" s="91" t="s">
+      <c r="F2" s="87" t="s">
         <v>406</v>
       </c>
-      <c r="G2" s="92" t="s">
+      <c r="G2" s="88" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="93">
+      <c r="A3" s="89">
         <v>1.2</v>
       </c>
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="90" t="s">
         <v>214</v>
       </c>
-      <c r="C3" s="95" t="s">
+      <c r="C3" s="91" t="s">
         <v>408</v>
       </c>
-      <c r="D3" s="95" t="s">
+      <c r="D3" s="91" t="s">
         <v>409</v>
       </c>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="91" t="s">
         <v>405</v>
       </c>
-      <c r="F3" s="95" t="s">
+      <c r="F3" s="91" t="s">
         <v>410</v>
       </c>
-      <c r="G3" s="96" t="s">
+      <c r="G3" s="92" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="63.75">
-      <c r="A4" s="93">
+      <c r="A4" s="89">
         <v>1.3</v>
       </c>
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="90" t="s">
         <v>412</v>
       </c>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="91" t="s">
         <v>413</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="D4" s="91" t="s">
         <v>414</v>
       </c>
-      <c r="E4" s="95" t="s">
+      <c r="E4" s="91" t="s">
         <v>415</v>
       </c>
-      <c r="F4" s="95" t="s">
+      <c r="F4" s="91" t="s">
         <v>416</v>
       </c>
-      <c r="G4" s="96" t="s">
+      <c r="G4" s="92" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="51">
-      <c r="A5" s="93">
+      <c r="A5" s="89">
         <v>1.4</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="90" t="s">
         <v>418</v>
       </c>
-      <c r="C5" s="95" t="s">
+      <c r="C5" s="91" t="s">
         <v>419</v>
       </c>
-      <c r="D5" s="95" t="s">
+      <c r="D5" s="91" t="s">
         <v>420</v>
       </c>
-      <c r="E5" s="95" t="s">
+      <c r="E5" s="91" t="s">
         <v>421</v>
       </c>
-      <c r="F5" s="95" t="s">
+      <c r="F5" s="91" t="s">
         <v>410</v>
       </c>
-      <c r="G5" s="96" t="s">
+      <c r="G5" s="92" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="38.25">
-      <c r="A6" s="93">
+      <c r="A6" s="89">
         <v>1.5</v>
       </c>
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="90" t="s">
         <v>423</v>
       </c>
-      <c r="C6" s="95" t="s">
+      <c r="C6" s="91" t="s">
         <v>424</v>
       </c>
-      <c r="D6" s="95" t="s">
+      <c r="D6" s="91" t="s">
         <v>425</v>
       </c>
-      <c r="E6" s="95" t="s">
+      <c r="E6" s="91" t="s">
         <v>426</v>
       </c>
-      <c r="F6" s="95" t="s">
+      <c r="F6" s="91" t="s">
         <v>416</v>
       </c>
-      <c r="G6" s="96" t="s">
+      <c r="G6" s="92" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="51">
-      <c r="A7" s="93">
+      <c r="A7" s="89">
         <v>2.1</v>
       </c>
-      <c r="B7" s="94" t="s">
+      <c r="B7" s="90" t="s">
         <v>428</v>
       </c>
-      <c r="C7" s="95" t="s">
+      <c r="C7" s="91" t="s">
         <v>429</v>
       </c>
-      <c r="D7" s="95" t="s">
+      <c r="D7" s="91" t="s">
         <v>430</v>
       </c>
-      <c r="E7" s="95" t="s">
+      <c r="E7" s="91" t="s">
         <v>431</v>
       </c>
-      <c r="F7" s="95" t="s">
+      <c r="F7" s="91" t="s">
         <v>406</v>
       </c>
-      <c r="G7" s="96" t="s">
+      <c r="G7" s="92" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="38.25">
-      <c r="A8" s="93">
+      <c r="A8" s="89">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B8" s="94" t="s">
+      <c r="B8" s="90" t="s">
         <v>433</v>
       </c>
-      <c r="C8" s="95" t="s">
+      <c r="C8" s="91" t="s">
         <v>434</v>
       </c>
-      <c r="D8" s="95" t="s">
+      <c r="D8" s="91" t="s">
         <v>435</v>
       </c>
-      <c r="E8" s="95" t="s">
+      <c r="E8" s="91" t="s">
         <v>405</v>
       </c>
-      <c r="F8" s="95" t="s">
+      <c r="F8" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="G8" s="96" t="s">
+      <c r="G8" s="92" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="38.25">
-      <c r="A9" s="93">
+      <c r="A9" s="89">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="90" t="s">
         <v>438</v>
       </c>
-      <c r="C9" s="95" t="s">
+      <c r="C9" s="91" t="s">
         <v>439</v>
       </c>
-      <c r="D9" s="95" t="s">
+      <c r="D9" s="91" t="s">
         <v>440</v>
       </c>
-      <c r="E9" s="95" t="s">
+      <c r="E9" s="91" t="s">
         <v>405</v>
       </c>
-      <c r="F9" s="95" t="s">
+      <c r="F9" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="G9" s="96" t="s">
+      <c r="G9" s="92" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="25.5">
-      <c r="A10" s="93">
+      <c r="A10" s="89">
         <v>2.4</v>
       </c>
-      <c r="B10" s="94" t="s">
+      <c r="B10" s="90" t="s">
         <v>441</v>
       </c>
-      <c r="C10" s="95" t="s">
+      <c r="C10" s="91" t="s">
         <v>442</v>
       </c>
-      <c r="D10" s="95" t="s">
+      <c r="D10" s="91" t="s">
         <v>443</v>
       </c>
-      <c r="E10" s="95" t="s">
+      <c r="E10" s="91" t="s">
         <v>444</v>
       </c>
-      <c r="F10" s="95" t="s">
+      <c r="F10" s="91" t="s">
         <v>406</v>
       </c>
-      <c r="G10" s="96" t="s">
+      <c r="G10" s="92" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="51">
-      <c r="A11" s="93">
+      <c r="A11" s="89">
         <v>3.1</v>
       </c>
-      <c r="B11" s="94" t="s">
+      <c r="B11" s="90" t="s">
         <v>446</v>
       </c>
-      <c r="C11" s="95" t="s">
+      <c r="C11" s="91" t="s">
         <v>447</v>
       </c>
-      <c r="D11" s="95" t="s">
+      <c r="D11" s="91" t="s">
         <v>448</v>
       </c>
-      <c r="E11" s="95" t="s">
+      <c r="E11" s="91" t="s">
         <v>449</v>
       </c>
-      <c r="F11" s="95" t="s">
+      <c r="F11" s="91" t="s">
         <v>416</v>
       </c>
-      <c r="G11" s="96" t="s">
+      <c r="G11" s="92" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="93">
+      <c r="A12" s="89">
         <v>3.2</v>
       </c>
-      <c r="B12" s="94" t="s">
+      <c r="B12" s="90" t="s">
         <v>451</v>
       </c>
-      <c r="C12" s="95" t="s">
+      <c r="C12" s="91" t="s">
         <v>452</v>
       </c>
-      <c r="D12" s="95" t="s">
+      <c r="D12" s="91" t="s">
         <v>440</v>
       </c>
-      <c r="E12" s="95" t="s">
+      <c r="E12" s="91" t="s">
         <v>405</v>
       </c>
-      <c r="F12" s="95" t="s">
+      <c r="F12" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="G12" s="96" t="s">
+      <c r="G12" s="92" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="25.5">
-      <c r="A13" s="93">
+      <c r="A13" s="89">
         <v>3.3</v>
       </c>
-      <c r="B13" s="94" t="s">
+      <c r="B13" s="90" t="s">
         <v>454</v>
       </c>
-      <c r="C13" s="95" t="s">
+      <c r="C13" s="91" t="s">
         <v>455</v>
       </c>
-      <c r="D13" s="95" t="s">
+      <c r="D13" s="91" t="s">
         <v>440</v>
       </c>
-      <c r="E13" s="95" t="s">
+      <c r="E13" s="91" t="s">
         <v>405</v>
       </c>
-      <c r="F13" s="95" t="s">
+      <c r="F13" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="G13" s="96" t="s">
+      <c r="G13" s="92" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="25.5">
-      <c r="A14" s="93">
+      <c r="A14" s="89">
         <v>3.4</v>
       </c>
-      <c r="B14" s="94" t="s">
+      <c r="B14" s="90" t="s">
         <v>456</v>
       </c>
-      <c r="C14" s="95" t="s">
+      <c r="C14" s="91" t="s">
         <v>457</v>
       </c>
-      <c r="D14" s="95" t="s">
+      <c r="D14" s="91" t="s">
         <v>440</v>
       </c>
-      <c r="E14" s="95" t="s">
+      <c r="E14" s="91" t="s">
         <v>405</v>
       </c>
-      <c r="F14" s="95" t="s">
+      <c r="F14" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="G14" s="96" t="s">
+      <c r="G14" s="92" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="76.5">
-      <c r="A15" s="93">
+      <c r="A15" s="89">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B15" s="94" t="s">
+      <c r="B15" s="90" t="s">
         <v>458</v>
       </c>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="91" t="s">
         <v>459</v>
       </c>
-      <c r="D15" s="95" t="s">
+      <c r="D15" s="91" t="s">
         <v>460</v>
       </c>
-      <c r="E15" s="95" t="s">
+      <c r="E15" s="91" t="s">
         <v>461</v>
       </c>
-      <c r="F15" s="95" t="s">
+      <c r="F15" s="91" t="s">
         <v>416</v>
       </c>
-      <c r="G15" s="96" t="s">
+      <c r="G15" s="92" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="25.5">
-      <c r="A16" s="93">
+      <c r="A16" s="89">
         <v>4.2</v>
       </c>
-      <c r="B16" s="94" t="s">
+      <c r="B16" s="90" t="s">
         <v>463</v>
       </c>
-      <c r="C16" s="95" t="s">
+      <c r="C16" s="91" t="s">
         <v>464</v>
       </c>
-      <c r="D16" s="95" t="s">
+      <c r="D16" s="91" t="s">
         <v>465</v>
       </c>
-      <c r="E16" s="95" t="s">
+      <c r="E16" s="91" t="s">
         <v>466</v>
       </c>
-      <c r="F16" s="95" t="s">
+      <c r="F16" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="G16" s="96" t="s">
+      <c r="G16" s="92" t="s">
         <v>467</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="25.5">
-      <c r="A17" s="93">
+      <c r="A17" s="89">
         <v>4.3</v>
       </c>
-      <c r="B17" s="94" t="s">
+      <c r="B17" s="90" t="s">
         <v>468</v>
       </c>
-      <c r="C17" s="95" t="s">
+      <c r="C17" s="91" t="s">
         <v>469</v>
       </c>
-      <c r="D17" s="95" t="s">
+      <c r="D17" s="91" t="s">
         <v>440</v>
       </c>
-      <c r="E17" s="95" t="s">
+      <c r="E17" s="91" t="s">
         <v>405</v>
       </c>
-      <c r="F17" s="95" t="s">
+      <c r="F17" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="G17" s="96" t="s">
+      <c r="G17" s="92" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="38.25">
-      <c r="A18" s="93">
+      <c r="A18" s="89">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B18" s="94" t="s">
+      <c r="B18" s="90" t="s">
         <v>470</v>
       </c>
-      <c r="C18" s="95" t="s">
+      <c r="C18" s="91" t="s">
         <v>471</v>
       </c>
-      <c r="D18" s="95" t="s">
+      <c r="D18" s="91" t="s">
         <v>465</v>
       </c>
-      <c r="E18" s="95" t="s">
+      <c r="E18" s="91" t="s">
         <v>472</v>
       </c>
-      <c r="F18" s="95" t="s">
+      <c r="F18" s="91" t="s">
         <v>416</v>
       </c>
-      <c r="G18" s="96" t="s">
+      <c r="G18" s="92" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="93">
+      <c r="A19" s="89">
         <v>4.5</v>
       </c>
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="90" t="s">
         <v>474</v>
       </c>
-      <c r="C19" s="95" t="s">
+      <c r="C19" s="91" t="s">
         <v>475</v>
       </c>
-      <c r="D19" s="95" t="s">
+      <c r="D19" s="91" t="s">
         <v>440</v>
       </c>
-      <c r="E19" s="95" t="s">
+      <c r="E19" s="91" t="s">
         <v>405</v>
       </c>
-      <c r="F19" s="95" t="s">
+      <c r="F19" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="G19" s="96" t="s">
+      <c r="G19" s="92" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="38.25">
-      <c r="A20" s="93">
+      <c r="A20" s="89">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B20" s="94" t="s">
+      <c r="B20" s="90" t="s">
         <v>476</v>
       </c>
-      <c r="C20" s="95" t="s">
+      <c r="C20" s="91" t="s">
         <v>477</v>
       </c>
-      <c r="D20" s="95" t="s">
+      <c r="D20" s="91" t="s">
         <v>440</v>
       </c>
-      <c r="E20" s="95" t="s">
+      <c r="E20" s="91" t="s">
         <v>405</v>
       </c>
-      <c r="F20" s="95" t="s">
+      <c r="F20" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="G20" s="96" t="s">
+      <c r="G20" s="92" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="25.5">
-      <c r="A21" s="93">
+      <c r="A21" s="89">
         <v>5.2</v>
       </c>
-      <c r="B21" s="94" t="s">
+      <c r="B21" s="90" t="s">
         <v>479</v>
       </c>
-      <c r="C21" s="95" t="s">
+      <c r="C21" s="91" t="s">
         <v>480</v>
       </c>
-      <c r="D21" s="95" t="s">
+      <c r="D21" s="91" t="s">
         <v>440</v>
       </c>
-      <c r="E21" s="95" t="s">
+      <c r="E21" s="91" t="s">
         <v>405</v>
       </c>
-      <c r="F21" s="95" t="s">
+      <c r="F21" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="G21" s="96" t="s">
+      <c r="G21" s="92" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="25.5">
-      <c r="A22" s="93">
+      <c r="A22" s="89">
         <v>5.3</v>
       </c>
-      <c r="B22" s="94" t="s">
+      <c r="B22" s="90" t="s">
         <v>481</v>
       </c>
-      <c r="C22" s="95" t="s">
+      <c r="C22" s="91" t="s">
         <v>482</v>
       </c>
-      <c r="D22" s="95" t="s">
+      <c r="D22" s="91" t="s">
         <v>440</v>
       </c>
-      <c r="E22" s="95" t="s">
+      <c r="E22" s="91" t="s">
         <v>405</v>
       </c>
-      <c r="F22" s="95" t="s">
+      <c r="F22" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="G22" s="96" t="s">
+      <c r="G22" s="92" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="25.5">
-      <c r="A23" s="93">
+      <c r="A23" s="89">
         <v>5.4</v>
       </c>
-      <c r="B23" s="94" t="s">
+      <c r="B23" s="90" t="s">
         <v>483</v>
       </c>
-      <c r="C23" s="95" t="s">
+      <c r="C23" s="91" t="s">
         <v>484</v>
       </c>
-      <c r="D23" s="95" t="s">
+      <c r="D23" s="91" t="s">
         <v>440</v>
       </c>
-      <c r="E23" s="95" t="s">
+      <c r="E23" s="91" t="s">
         <v>405</v>
       </c>
-      <c r="F23" s="95" t="s">
+      <c r="F23" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="G23" s="96" t="s">
+      <c r="G23" s="92" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="25.5">
-      <c r="A24" s="93">
+      <c r="A24" s="89">
         <v>6.1</v>
       </c>
-      <c r="B24" s="94" t="s">
+      <c r="B24" s="90" t="s">
         <v>485</v>
       </c>
-      <c r="C24" s="95" t="s">
+      <c r="C24" s="91" t="s">
         <v>486</v>
       </c>
-      <c r="D24" s="95" t="s">
+      <c r="D24" s="91" t="s">
         <v>440</v>
       </c>
-      <c r="E24" s="95" t="s">
+      <c r="E24" s="91" t="s">
         <v>405</v>
       </c>
-      <c r="F24" s="95" t="s">
+      <c r="F24" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="G24" s="96" t="s">
+      <c r="G24" s="92" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="25.5">
-      <c r="A25" s="93">
+      <c r="A25" s="89">
         <v>7.1</v>
       </c>
-      <c r="B25" s="94" t="s">
+      <c r="B25" s="90" t="s">
         <v>487</v>
       </c>
-      <c r="C25" s="95" t="s">
+      <c r="C25" s="91" t="s">
         <v>488</v>
       </c>
-      <c r="D25" s="95" t="s">
+      <c r="D25" s="91" t="s">
         <v>440</v>
       </c>
-      <c r="E25" s="95" t="s">
+      <c r="E25" s="91" t="s">
         <v>405</v>
       </c>
-      <c r="F25" s="95" t="s">
+      <c r="F25" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="G25" s="96" t="s">
+      <c r="G25" s="92" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="93">
+      <c r="A26" s="89">
         <v>7.2</v>
       </c>
-      <c r="B26" s="94" t="s">
+      <c r="B26" s="90" t="s">
         <v>489</v>
       </c>
-      <c r="C26" s="95" t="s">
+      <c r="C26" s="91" t="s">
         <v>490</v>
       </c>
-      <c r="D26" s="95" t="s">
+      <c r="D26" s="91" t="s">
         <v>440</v>
       </c>
-      <c r="E26" s="95" t="s">
+      <c r="E26" s="91" t="s">
         <v>405</v>
       </c>
-      <c r="F26" s="95" t="s">
+      <c r="F26" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="G26" s="96" t="s">
+      <c r="G26" s="92" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="25.5">
-      <c r="A27" s="93">
+      <c r="A27" s="89">
         <v>7.3</v>
       </c>
-      <c r="B27" s="94" t="s">
+      <c r="B27" s="90" t="s">
         <v>491</v>
       </c>
-      <c r="C27" s="95" t="s">
+      <c r="C27" s="91" t="s">
         <v>492</v>
       </c>
-      <c r="D27" s="95" t="s">
+      <c r="D27" s="91" t="s">
         <v>440</v>
       </c>
-      <c r="E27" s="95" t="s">
+      <c r="E27" s="91" t="s">
         <v>405</v>
       </c>
-      <c r="F27" s="95" t="s">
+      <c r="F27" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="G27" s="96" t="s">
+      <c r="G27" s="92" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="25.5">
-      <c r="A28" s="93" t="s">
+      <c r="A28" s="89" t="s">
         <v>493</v>
       </c>
-      <c r="B28" s="94" t="s">
+      <c r="B28" s="90" t="s">
         <v>494</v>
       </c>
-      <c r="C28" s="95" t="s">
+      <c r="C28" s="91" t="s">
         <v>495</v>
       </c>
-      <c r="D28" s="95" t="s">
+      <c r="D28" s="91" t="s">
         <v>496</v>
       </c>
-      <c r="E28" s="95" t="s">
+      <c r="E28" s="91" t="s">
         <v>405</v>
       </c>
-      <c r="F28" s="95" t="s">
+      <c r="F28" s="91" t="s">
         <v>406</v>
       </c>
-      <c r="G28" s="96" t="s">
+      <c r="G28" s="92" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="25.5">
-      <c r="A29" s="93" t="s">
+      <c r="A29" s="89" t="s">
         <v>493</v>
       </c>
-      <c r="B29" s="94" t="s">
+      <c r="B29" s="90" t="s">
         <v>498</v>
       </c>
-      <c r="C29" s="95" t="s">
+      <c r="C29" s="91" t="s">
         <v>499</v>
       </c>
-      <c r="D29" s="95" t="s">
+      <c r="D29" s="91" t="s">
         <v>500</v>
       </c>
-      <c r="E29" s="95" t="s">
+      <c r="E29" s="91" t="s">
         <v>501</v>
       </c>
-      <c r="F29" s="95" t="s">
+      <c r="F29" s="91" t="s">
         <v>406</v>
       </c>
-      <c r="G29" s="96" t="s">
+      <c r="G29" s="92" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="25.5">
-      <c r="A30" s="93" t="s">
+      <c r="A30" s="89" t="s">
         <v>493</v>
       </c>
-      <c r="B30" s="94" t="s">
+      <c r="B30" s="90" t="s">
         <v>502</v>
       </c>
-      <c r="C30" s="95" t="s">
+      <c r="C30" s="91" t="s">
         <v>503</v>
       </c>
-      <c r="D30" s="95" t="s">
+      <c r="D30" s="91" t="s">
         <v>500</v>
       </c>
-      <c r="E30" s="95" t="s">
+      <c r="E30" s="91" t="s">
         <v>504</v>
       </c>
-      <c r="F30" s="95" t="s">
+      <c r="F30" s="91" t="s">
         <v>505</v>
       </c>
-      <c r="G30" s="96" t="s">
+      <c r="G30" s="92" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="38.25">
-      <c r="A31" s="93" t="s">
+      <c r="A31" s="89" t="s">
         <v>493</v>
       </c>
-      <c r="B31" s="94" t="s">
+      <c r="B31" s="90" t="s">
         <v>506</v>
       </c>
-      <c r="C31" s="95" t="s">
+      <c r="C31" s="91" t="s">
         <v>507</v>
       </c>
-      <c r="D31" s="95" t="s">
+      <c r="D31" s="91" t="s">
         <v>500</v>
       </c>
-      <c r="E31" s="95" t="s">
+      <c r="E31" s="91" t="s">
         <v>508</v>
       </c>
-      <c r="F31" s="95" t="s">
+      <c r="F31" s="91" t="s">
         <v>505</v>
       </c>
-      <c r="G31" s="96" t="s">
+      <c r="G31" s="92" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="38.25">
-      <c r="A32" s="93" t="s">
+      <c r="A32" s="89" t="s">
         <v>509</v>
       </c>
-      <c r="B32" s="94" t="s">
+      <c r="B32" s="90" t="s">
         <v>510</v>
       </c>
-      <c r="C32" s="95" t="s">
+      <c r="C32" s="91" t="s">
         <v>511</v>
       </c>
-      <c r="D32" s="95" t="s">
+      <c r="D32" s="91" t="s">
         <v>512</v>
       </c>
-      <c r="E32" s="95" t="s">
+      <c r="E32" s="91" t="s">
         <v>513</v>
       </c>
-      <c r="F32" s="95" t="s">
+      <c r="F32" s="91" t="s">
         <v>436</v>
       </c>
-      <c r="G32" s="96" t="s">
+      <c r="G32" s="92" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="51.75" thickBot="1">
-      <c r="A33" s="97" t="s">
+      <c r="A33" s="93" t="s">
         <v>509</v>
       </c>
-      <c r="B33" s="98" t="s">
+      <c r="B33" s="94" t="s">
         <v>515</v>
       </c>
-      <c r="C33" s="99" t="s">
+      <c r="C33" s="95" t="s">
         <v>516</v>
       </c>
-      <c r="D33" s="99" t="s">
+      <c r="D33" s="95" t="s">
         <v>517</v>
       </c>
-      <c r="E33" s="99" t="s">
+      <c r="E33" s="95" t="s">
         <v>518</v>
       </c>
-      <c r="F33" s="99" t="s">
+      <c r="F33" s="95" t="s">
         <v>436</v>
       </c>
-      <c r="G33" s="100" t="s">
+      <c r="G33" s="96" t="s">
         <v>519</v>
       </c>
     </row>
@@ -7650,818 +7783,818 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.7109375" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="114" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="114" customWidth="1"/>
-    <col min="3" max="3" width="98.85546875" style="114" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="114" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="114" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="114" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="114" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="114" customWidth="1"/>
-    <col min="9" max="16384" width="11.7109375" style="114"/>
+    <col min="1" max="1" width="21.28515625" style="110" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="110" customWidth="1"/>
+    <col min="3" max="3" width="98.85546875" style="110" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="110" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="110" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="110" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="110" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" style="110" customWidth="1"/>
+    <col min="9" max="16384" width="11.7109375" style="110"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A1" s="205" t="s">
+      <c r="A1" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="B1" s="206"/>
-      <c r="C1" s="116" t="s">
+      <c r="B1" s="197"/>
+      <c r="C1" s="112" t="s">
         <v>272</v>
       </c>
-      <c r="D1" s="116" t="s">
+      <c r="D1" s="112" t="s">
         <v>273</v>
       </c>
-      <c r="E1" s="116" t="s">
+      <c r="E1" s="112" t="s">
         <v>520</v>
       </c>
-      <c r="F1" s="116" t="s">
+      <c r="F1" s="112" t="s">
         <v>521</v>
       </c>
-      <c r="G1" s="116" t="s">
+      <c r="G1" s="112" t="s">
         <v>522</v>
       </c>
-      <c r="H1" s="117" t="s">
+      <c r="H1" s="113" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="108" t="s">
         <v>524</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="113"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="109"/>
     </row>
     <row r="3" spans="1:8" ht="67.5" customHeight="1">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="101" t="s">
         <v>275</v>
       </c>
-      <c r="B3" s="103" t="s">
+      <c r="B3" s="99" t="s">
         <v>402</v>
       </c>
-      <c r="C3" s="103" t="s">
+      <c r="C3" s="99" t="s">
         <v>276</v>
       </c>
-      <c r="D3" s="103" t="s">
+      <c r="D3" s="99" t="s">
         <v>277</v>
       </c>
-      <c r="E3" s="103" t="s">
+      <c r="E3" s="99" t="s">
         <v>525</v>
       </c>
-      <c r="F3" s="103" t="s">
+      <c r="F3" s="99" t="s">
         <v>526</v>
       </c>
-      <c r="G3" s="103"/>
-      <c r="H3" s="106" t="s">
+      <c r="G3" s="99"/>
+      <c r="H3" s="102" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45" customHeight="1">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="101" t="s">
         <v>278</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="99" t="s">
         <v>214</v>
       </c>
-      <c r="C4" s="103" t="s">
+      <c r="C4" s="99" t="s">
         <v>279</v>
       </c>
-      <c r="D4" s="103" t="s">
+      <c r="D4" s="99" t="s">
         <v>280</v>
       </c>
-      <c r="E4" s="103" t="s">
+      <c r="E4" s="99" t="s">
         <v>528</v>
       </c>
-      <c r="F4" s="103" t="s">
+      <c r="F4" s="99" t="s">
         <v>529</v>
       </c>
-      <c r="G4" s="103"/>
-      <c r="H4" s="106" t="s">
+      <c r="G4" s="99"/>
+      <c r="H4" s="102" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="78.75" customHeight="1">
-      <c r="A5" s="105" t="s">
+      <c r="A5" s="101" t="s">
         <v>281</v>
       </c>
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="99" t="s">
         <v>412</v>
       </c>
-      <c r="C5" s="103" t="s">
+      <c r="C5" s="99" t="s">
         <v>282</v>
       </c>
-      <c r="D5" s="103" t="s">
+      <c r="D5" s="99" t="s">
         <v>283</v>
       </c>
-      <c r="E5" s="103" t="s">
+      <c r="E5" s="99" t="s">
         <v>531</v>
       </c>
-      <c r="F5" s="103" t="s">
+      <c r="F5" s="99" t="s">
         <v>532</v>
       </c>
-      <c r="G5" s="103"/>
-      <c r="H5" s="106" t="s">
+      <c r="G5" s="99"/>
+      <c r="H5" s="102" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A6" s="105" t="s">
+      <c r="A6" s="101" t="s">
         <v>284</v>
       </c>
-      <c r="B6" s="103" t="s">
+      <c r="B6" s="99" t="s">
         <v>418</v>
       </c>
-      <c r="C6" s="103" t="s">
+      <c r="C6" s="99" t="s">
         <v>285</v>
       </c>
-      <c r="D6" s="103" t="s">
+      <c r="D6" s="99" t="s">
         <v>286</v>
       </c>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103" t="s">
+      <c r="E6" s="99"/>
+      <c r="F6" s="99" t="s">
         <v>534</v>
       </c>
-      <c r="G6" s="103"/>
-      <c r="H6" s="106" t="s">
+      <c r="G6" s="99"/>
+      <c r="H6" s="102" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A7" s="105" t="s">
+      <c r="A7" s="101" t="s">
         <v>287</v>
       </c>
-      <c r="B7" s="103" t="s">
+      <c r="B7" s="99" t="s">
         <v>423</v>
       </c>
-      <c r="C7" s="103" t="s">
+      <c r="C7" s="99" t="s">
         <v>288</v>
       </c>
-      <c r="D7" s="103" t="s">
+      <c r="D7" s="99" t="s">
         <v>289</v>
       </c>
-      <c r="E7" s="103" t="s">
+      <c r="E7" s="99" t="s">
         <v>536</v>
       </c>
-      <c r="F7" s="103" t="s">
+      <c r="F7" s="99" t="s">
         <v>537</v>
       </c>
-      <c r="G7" s="103"/>
-      <c r="H7" s="106" t="s">
+      <c r="G7" s="99"/>
+      <c r="H7" s="102" t="s">
         <v>538</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A8" s="111" t="s">
+      <c r="A8" s="107" t="s">
         <v>290</v>
       </c>
-      <c r="B8" s="112" t="s">
+      <c r="B8" s="108" t="s">
         <v>539</v>
       </c>
-      <c r="C8" s="112"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="113"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="108"/>
+      <c r="E8" s="108"/>
+      <c r="F8" s="108"/>
+      <c r="G8" s="108"/>
+      <c r="H8" s="109"/>
     </row>
     <row r="9" spans="1:8" ht="67.5" customHeight="1">
-      <c r="A9" s="105" t="s">
+      <c r="A9" s="101" t="s">
         <v>291</v>
       </c>
-      <c r="B9" s="103" t="s">
+      <c r="B9" s="99" t="s">
         <v>428</v>
       </c>
-      <c r="C9" s="103" t="s">
+      <c r="C9" s="99" t="s">
         <v>292</v>
       </c>
-      <c r="D9" s="103" t="s">
+      <c r="D9" s="99" t="s">
         <v>293</v>
       </c>
-      <c r="E9" s="103" t="s">
+      <c r="E9" s="99" t="s">
         <v>540</v>
       </c>
-      <c r="F9" s="103" t="s">
+      <c r="F9" s="99" t="s">
         <v>541</v>
       </c>
-      <c r="G9" s="103"/>
-      <c r="H9" s="106" t="s">
+      <c r="G9" s="99"/>
+      <c r="H9" s="102" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A10" s="105" t="s">
+      <c r="A10" s="101" t="s">
         <v>294</v>
       </c>
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="99" t="s">
         <v>543</v>
       </c>
-      <c r="C10" s="103" t="s">
+      <c r="C10" s="99" t="s">
         <v>295</v>
       </c>
-      <c r="D10" s="103" t="s">
+      <c r="D10" s="99" t="s">
         <v>296</v>
       </c>
-      <c r="E10" s="103"/>
-      <c r="F10" s="103" t="s">
+      <c r="E10" s="99"/>
+      <c r="F10" s="99" t="s">
         <v>544</v>
       </c>
-      <c r="G10" s="103"/>
-      <c r="H10" s="106" t="s">
+      <c r="G10" s="99"/>
+      <c r="H10" s="102" t="s">
         <v>545</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A11" s="105" t="s">
+      <c r="A11" s="101" t="s">
         <v>297</v>
       </c>
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="99" t="s">
         <v>546</v>
       </c>
-      <c r="C11" s="103" t="s">
+      <c r="C11" s="99" t="s">
         <v>298</v>
       </c>
-      <c r="D11" s="103" t="s">
+      <c r="D11" s="99" t="s">
         <v>299</v>
       </c>
-      <c r="E11" s="103" t="s">
+      <c r="E11" s="99" t="s">
         <v>547</v>
       </c>
-      <c r="F11" s="103" t="s">
+      <c r="F11" s="99" t="s">
         <v>548</v>
       </c>
-      <c r="G11" s="103"/>
-      <c r="H11" s="106" t="s">
+      <c r="G11" s="99"/>
+      <c r="H11" s="102" t="s">
         <v>549</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A12" s="105" t="s">
+      <c r="A12" s="101" t="s">
         <v>300</v>
       </c>
-      <c r="B12" s="103" t="s">
+      <c r="B12" s="99" t="s">
         <v>441</v>
       </c>
-      <c r="C12" s="103" t="s">
+      <c r="C12" s="99" t="s">
         <v>301</v>
       </c>
-      <c r="D12" s="103" t="s">
+      <c r="D12" s="99" t="s">
         <v>302</v>
       </c>
-      <c r="E12" s="103"/>
-      <c r="F12" s="103" t="s">
+      <c r="E12" s="99"/>
+      <c r="F12" s="99" t="s">
         <v>550</v>
       </c>
-      <c r="G12" s="103"/>
-      <c r="H12" s="106" t="s">
+      <c r="G12" s="99"/>
+      <c r="H12" s="102" t="s">
         <v>551</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A13" s="111" t="s">
+      <c r="A13" s="107" t="s">
         <v>303</v>
       </c>
-      <c r="B13" s="112" t="s">
+      <c r="B13" s="108" t="s">
         <v>552</v>
       </c>
-      <c r="C13" s="112"/>
-      <c r="D13" s="112"/>
-      <c r="E13" s="112"/>
-      <c r="F13" s="112"/>
-      <c r="G13" s="112"/>
-      <c r="H13" s="113"/>
+      <c r="C13" s="108"/>
+      <c r="D13" s="108"/>
+      <c r="E13" s="108"/>
+      <c r="F13" s="108"/>
+      <c r="G13" s="108"/>
+      <c r="H13" s="109"/>
     </row>
     <row r="14" spans="1:8" ht="67.5" customHeight="1">
-      <c r="A14" s="105" t="s">
+      <c r="A14" s="101" t="s">
         <v>304</v>
       </c>
-      <c r="B14" s="103" t="s">
+      <c r="B14" s="99" t="s">
         <v>446</v>
       </c>
-      <c r="C14" s="103" t="s">
+      <c r="C14" s="99" t="s">
         <v>603</v>
       </c>
-      <c r="D14" s="103" t="s">
+      <c r="D14" s="99" t="s">
         <v>305</v>
       </c>
-      <c r="E14" s="103" t="s">
+      <c r="E14" s="99" t="s">
         <v>553</v>
       </c>
-      <c r="F14" s="103" t="s">
+      <c r="F14" s="99" t="s">
         <v>554</v>
       </c>
-      <c r="G14" s="103"/>
-      <c r="H14" s="106" t="s">
+      <c r="G14" s="99"/>
+      <c r="H14" s="102" t="s">
         <v>555</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="56.25" customHeight="1">
-      <c r="A15" s="105" t="s">
+      <c r="A15" s="101" t="s">
         <v>306</v>
       </c>
-      <c r="B15" s="103" t="s">
+      <c r="B15" s="99" t="s">
         <v>451</v>
       </c>
-      <c r="C15" s="103" t="s">
+      <c r="C15" s="99" t="s">
         <v>307</v>
       </c>
-      <c r="D15" s="103" t="s">
+      <c r="D15" s="99" t="s">
         <v>308</v>
       </c>
-      <c r="E15" s="103" t="s">
+      <c r="E15" s="99" t="s">
         <v>556</v>
       </c>
-      <c r="F15" s="103" t="s">
+      <c r="F15" s="99" t="s">
         <v>557</v>
       </c>
-      <c r="G15" s="103"/>
-      <c r="H15" s="106" t="s">
+      <c r="G15" s="99"/>
+      <c r="H15" s="102" t="s">
         <v>558</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A16" s="105" t="s">
+      <c r="A16" s="101" t="s">
         <v>309</v>
       </c>
-      <c r="B16" s="103" t="s">
+      <c r="B16" s="99" t="s">
         <v>454</v>
       </c>
-      <c r="C16" s="103" t="s">
+      <c r="C16" s="99" t="s">
         <v>310</v>
       </c>
-      <c r="D16" s="103" t="s">
+      <c r="D16" s="99" t="s">
         <v>311</v>
       </c>
-      <c r="E16" s="103"/>
-      <c r="F16" s="103" t="s">
+      <c r="E16" s="99"/>
+      <c r="F16" s="99" t="s">
         <v>559</v>
       </c>
-      <c r="G16" s="103"/>
-      <c r="H16" s="106" t="s">
+      <c r="G16" s="99"/>
+      <c r="H16" s="102" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1">
-      <c r="A17" s="105" t="s">
+      <c r="A17" s="101" t="s">
         <v>312</v>
       </c>
-      <c r="B17" s="103" t="s">
+      <c r="B17" s="99" t="s">
         <v>456</v>
       </c>
-      <c r="C17" s="103" t="s">
+      <c r="C17" s="99" t="s">
         <v>313</v>
       </c>
-      <c r="D17" s="103" t="s">
+      <c r="D17" s="99" t="s">
         <v>314</v>
       </c>
-      <c r="E17" s="103"/>
-      <c r="F17" s="103" t="s">
+      <c r="E17" s="99"/>
+      <c r="F17" s="99" t="s">
         <v>561</v>
       </c>
-      <c r="G17" s="103"/>
-      <c r="H17" s="106" t="s">
+      <c r="G17" s="99"/>
+      <c r="H17" s="102" t="s">
         <v>562</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A18" s="111" t="s">
+      <c r="A18" s="107" t="s">
         <v>315</v>
       </c>
-      <c r="B18" s="112" t="s">
+      <c r="B18" s="108" t="s">
         <v>563</v>
       </c>
-      <c r="C18" s="112"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="112"/>
-      <c r="F18" s="112"/>
-      <c r="G18" s="112"/>
-      <c r="H18" s="113"/>
+      <c r="C18" s="108"/>
+      <c r="D18" s="108"/>
+      <c r="E18" s="108"/>
+      <c r="F18" s="108"/>
+      <c r="G18" s="108"/>
+      <c r="H18" s="109"/>
     </row>
     <row r="19" spans="1:8" ht="67.5" customHeight="1">
-      <c r="A19" s="105" t="s">
+      <c r="A19" s="101" t="s">
         <v>316</v>
       </c>
-      <c r="B19" s="103" t="s">
+      <c r="B19" s="99" t="s">
         <v>458</v>
       </c>
-      <c r="C19" s="103" t="s">
+      <c r="C19" s="99" t="s">
         <v>317</v>
       </c>
-      <c r="D19" s="103" t="s">
+      <c r="D19" s="99" t="s">
         <v>318</v>
       </c>
-      <c r="E19" s="103" t="s">
+      <c r="E19" s="99" t="s">
         <v>564</v>
       </c>
-      <c r="F19" s="103" t="s">
+      <c r="F19" s="99" t="s">
         <v>565</v>
       </c>
-      <c r="G19" s="103"/>
-      <c r="H19" s="106" t="s">
+      <c r="G19" s="99"/>
+      <c r="H19" s="102" t="s">
         <v>566</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="45" customHeight="1">
-      <c r="A20" s="105" t="s">
+      <c r="A20" s="101" t="s">
         <v>319</v>
       </c>
-      <c r="B20" s="103" t="s">
+      <c r="B20" s="99" t="s">
         <v>463</v>
       </c>
-      <c r="C20" s="103" t="s">
+      <c r="C20" s="99" t="s">
         <v>320</v>
       </c>
-      <c r="D20" s="103" t="s">
+      <c r="D20" s="99" t="s">
         <v>321</v>
       </c>
-      <c r="E20" s="103" t="s">
+      <c r="E20" s="99" t="s">
         <v>564</v>
       </c>
-      <c r="F20" s="103" t="s">
+      <c r="F20" s="99" t="s">
         <v>567</v>
       </c>
-      <c r="G20" s="103"/>
-      <c r="H20" s="106" t="s">
+      <c r="G20" s="99"/>
+      <c r="H20" s="102" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A21" s="105" t="s">
+      <c r="A21" s="101" t="s">
         <v>322</v>
       </c>
-      <c r="B21" s="103" t="s">
+      <c r="B21" s="99" t="s">
         <v>569</v>
       </c>
-      <c r="C21" s="103" t="s">
+      <c r="C21" s="99" t="s">
         <v>323</v>
       </c>
-      <c r="D21" s="103" t="s">
+      <c r="D21" s="99" t="s">
         <v>324</v>
       </c>
-      <c r="E21" s="103" t="s">
+      <c r="E21" s="99" t="s">
         <v>570</v>
       </c>
-      <c r="F21" s="103" t="s">
+      <c r="F21" s="99" t="s">
         <v>571</v>
       </c>
-      <c r="G21" s="103"/>
-      <c r="H21" s="106" t="s">
+      <c r="G21" s="99"/>
+      <c r="H21" s="102" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="112.5" customHeight="1">
-      <c r="A22" s="105" t="s">
+      <c r="A22" s="101" t="s">
         <v>325</v>
       </c>
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="99" t="s">
         <v>470</v>
       </c>
-      <c r="C22" s="103" t="s">
+      <c r="C22" s="99" t="s">
         <v>604</v>
       </c>
-      <c r="D22" s="103" t="s">
+      <c r="D22" s="99" t="s">
         <v>326</v>
       </c>
-      <c r="E22" s="103"/>
-      <c r="F22" s="103" t="s">
+      <c r="E22" s="99"/>
+      <c r="F22" s="99" t="s">
         <v>573</v>
       </c>
-      <c r="G22" s="103"/>
-      <c r="H22" s="106" t="s">
+      <c r="G22" s="99"/>
+      <c r="H22" s="102" t="s">
         <v>574</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A23" s="105" t="s">
+      <c r="A23" s="101" t="s">
         <v>327</v>
       </c>
-      <c r="B23" s="103" t="s">
+      <c r="B23" s="99" t="s">
         <v>474</v>
       </c>
-      <c r="C23" s="103" t="s">
+      <c r="C23" s="99" t="s">
         <v>328</v>
       </c>
-      <c r="D23" s="103" t="s">
+      <c r="D23" s="99" t="s">
         <v>329</v>
       </c>
-      <c r="E23" s="103"/>
-      <c r="F23" s="103" t="s">
+      <c r="E23" s="99"/>
+      <c r="F23" s="99" t="s">
         <v>575</v>
       </c>
-      <c r="G23" s="103"/>
-      <c r="H23" s="106" t="s">
+      <c r="G23" s="99"/>
+      <c r="H23" s="102" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A24" s="111" t="s">
+      <c r="A24" s="107" t="s">
         <v>330</v>
       </c>
-      <c r="B24" s="112" t="s">
+      <c r="B24" s="108" t="s">
         <v>577</v>
       </c>
-      <c r="C24" s="112"/>
-      <c r="D24" s="112"/>
-      <c r="E24" s="112"/>
-      <c r="F24" s="112"/>
-      <c r="G24" s="112"/>
-      <c r="H24" s="113"/>
+      <c r="C24" s="108"/>
+      <c r="D24" s="108"/>
+      <c r="E24" s="108"/>
+      <c r="F24" s="108"/>
+      <c r="G24" s="108"/>
+      <c r="H24" s="109"/>
     </row>
     <row r="25" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A25" s="105" t="s">
+      <c r="A25" s="101" t="s">
         <v>331</v>
       </c>
-      <c r="B25" s="103" t="s">
+      <c r="B25" s="99" t="s">
         <v>476</v>
       </c>
-      <c r="C25" s="103" t="s">
+      <c r="C25" s="99" t="s">
         <v>332</v>
       </c>
-      <c r="D25" s="103" t="s">
+      <c r="D25" s="99" t="s">
         <v>333</v>
       </c>
-      <c r="E25" s="103" t="s">
+      <c r="E25" s="99" t="s">
         <v>578</v>
       </c>
-      <c r="F25" s="103" t="s">
+      <c r="F25" s="99" t="s">
         <v>579</v>
       </c>
-      <c r="G25" s="103"/>
-      <c r="H25" s="106" t="s">
+      <c r="G25" s="99"/>
+      <c r="H25" s="102" t="s">
         <v>580</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A26" s="105" t="s">
+      <c r="A26" s="101" t="s">
         <v>334</v>
       </c>
-      <c r="B26" s="103" t="s">
+      <c r="B26" s="99" t="s">
         <v>479</v>
       </c>
-      <c r="C26" s="103" t="s">
+      <c r="C26" s="99" t="s">
         <v>335</v>
       </c>
-      <c r="D26" s="103" t="s">
+      <c r="D26" s="99" t="s">
         <v>336</v>
       </c>
-      <c r="E26" s="103"/>
-      <c r="F26" s="103" t="s">
+      <c r="E26" s="99"/>
+      <c r="F26" s="99" t="s">
         <v>581</v>
       </c>
-      <c r="G26" s="103"/>
-      <c r="H26" s="106" t="s">
+      <c r="G26" s="99"/>
+      <c r="H26" s="102" t="s">
         <v>580</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A27" s="105" t="s">
+      <c r="A27" s="101" t="s">
         <v>337</v>
       </c>
-      <c r="B27" s="103" t="s">
+      <c r="B27" s="99" t="s">
         <v>481</v>
       </c>
-      <c r="C27" s="103" t="s">
+      <c r="C27" s="99" t="s">
         <v>338</v>
       </c>
-      <c r="D27" s="103" t="s">
+      <c r="D27" s="99" t="s">
         <v>339</v>
       </c>
-      <c r="E27" s="103"/>
-      <c r="F27" s="103" t="s">
+      <c r="E27" s="99"/>
+      <c r="F27" s="99" t="s">
         <v>582</v>
       </c>
-      <c r="G27" s="103"/>
-      <c r="H27" s="106" t="s">
+      <c r="G27" s="99"/>
+      <c r="H27" s="102" t="s">
         <v>583</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A28" s="105" t="s">
+      <c r="A28" s="101" t="s">
         <v>340</v>
       </c>
-      <c r="B28" s="103" t="s">
+      <c r="B28" s="99" t="s">
         <v>483</v>
       </c>
-      <c r="C28" s="103" t="s">
+      <c r="C28" s="99" t="s">
         <v>341</v>
       </c>
-      <c r="D28" s="103" t="s">
+      <c r="D28" s="99" t="s">
         <v>342</v>
       </c>
-      <c r="E28" s="103"/>
-      <c r="F28" s="103" t="s">
+      <c r="E28" s="99"/>
+      <c r="F28" s="99" t="s">
         <v>584</v>
       </c>
-      <c r="G28" s="103"/>
-      <c r="H28" s="106"/>
+      <c r="G28" s="99"/>
+      <c r="H28" s="102"/>
     </row>
     <row r="29" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A29" s="111" t="s">
+      <c r="A29" s="107" t="s">
         <v>343</v>
       </c>
-      <c r="B29" s="112" t="s">
+      <c r="B29" s="108" t="s">
         <v>585</v>
       </c>
-      <c r="C29" s="112"/>
-      <c r="D29" s="112"/>
-      <c r="E29" s="112"/>
-      <c r="F29" s="112"/>
-      <c r="G29" s="112"/>
-      <c r="H29" s="113"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="108"/>
+      <c r="E29" s="108"/>
+      <c r="F29" s="108"/>
+      <c r="G29" s="108"/>
+      <c r="H29" s="109"/>
     </row>
     <row r="30" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A30" s="105" t="s">
+      <c r="A30" s="101" t="s">
         <v>344</v>
       </c>
-      <c r="B30" s="103" t="s">
+      <c r="B30" s="99" t="s">
         <v>485</v>
       </c>
-      <c r="C30" s="103" t="s">
+      <c r="C30" s="99" t="s">
         <v>345</v>
       </c>
-      <c r="D30" s="103" t="s">
+      <c r="D30" s="99" t="s">
         <v>346</v>
       </c>
-      <c r="E30" s="103"/>
-      <c r="F30" s="103" t="s">
+      <c r="E30" s="99"/>
+      <c r="F30" s="99" t="s">
         <v>586</v>
       </c>
-      <c r="G30" s="103"/>
-      <c r="H30" s="106" t="s">
+      <c r="G30" s="99"/>
+      <c r="H30" s="102" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A31" s="111" t="s">
+      <c r="A31" s="107" t="s">
         <v>347</v>
       </c>
-      <c r="B31" s="112" t="s">
+      <c r="B31" s="108" t="s">
         <v>588</v>
       </c>
-      <c r="C31" s="112"/>
-      <c r="D31" s="112"/>
-      <c r="E31" s="112"/>
-      <c r="F31" s="112"/>
-      <c r="G31" s="112"/>
-      <c r="H31" s="113"/>
+      <c r="C31" s="108"/>
+      <c r="D31" s="108"/>
+      <c r="E31" s="108"/>
+      <c r="F31" s="108"/>
+      <c r="G31" s="108"/>
+      <c r="H31" s="109"/>
     </row>
     <row r="32" spans="1:8" ht="45" customHeight="1">
-      <c r="A32" s="105" t="s">
+      <c r="A32" s="101" t="s">
         <v>348</v>
       </c>
-      <c r="B32" s="103" t="s">
+      <c r="B32" s="99" t="s">
         <v>589</v>
       </c>
-      <c r="C32" s="103" t="s">
+      <c r="C32" s="99" t="s">
         <v>349</v>
       </c>
-      <c r="D32" s="103" t="s">
+      <c r="D32" s="99" t="s">
         <v>350</v>
       </c>
-      <c r="E32" s="103"/>
-      <c r="F32" s="103" t="s">
+      <c r="E32" s="99"/>
+      <c r="F32" s="99" t="s">
         <v>590</v>
       </c>
-      <c r="G32" s="103"/>
-      <c r="H32" s="106" t="s">
+      <c r="G32" s="99"/>
+      <c r="H32" s="102" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A33" s="105" t="s">
+      <c r="A33" s="101" t="s">
         <v>351</v>
       </c>
-      <c r="B33" s="103" t="s">
+      <c r="B33" s="99" t="s">
         <v>489</v>
       </c>
-      <c r="C33" s="103" t="s">
+      <c r="C33" s="99" t="s">
         <v>352</v>
       </c>
-      <c r="D33" s="103" t="s">
+      <c r="D33" s="99" t="s">
         <v>353</v>
       </c>
-      <c r="E33" s="103"/>
-      <c r="F33" s="103" t="s">
+      <c r="E33" s="99"/>
+      <c r="F33" s="99" t="s">
         <v>592</v>
       </c>
-      <c r="G33" s="103"/>
-      <c r="H33" s="106"/>
+      <c r="G33" s="99"/>
+      <c r="H33" s="102"/>
     </row>
     <row r="34" spans="1:8" ht="23.25" customHeight="1">
-      <c r="A34" s="105" t="s">
+      <c r="A34" s="101" t="s">
         <v>354</v>
       </c>
-      <c r="B34" s="103" t="s">
+      <c r="B34" s="99" t="s">
         <v>491</v>
       </c>
-      <c r="C34" s="103" t="s">
+      <c r="C34" s="99" t="s">
         <v>352</v>
       </c>
-      <c r="D34" s="103" t="s">
+      <c r="D34" s="99" t="s">
         <v>355</v>
       </c>
-      <c r="E34" s="103"/>
-      <c r="F34" s="103" t="s">
+      <c r="E34" s="99"/>
+      <c r="F34" s="99" t="s">
         <v>593</v>
       </c>
-      <c r="G34" s="103"/>
-      <c r="H34" s="106" t="s">
+      <c r="G34" s="99"/>
+      <c r="H34" s="102" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A35" s="104"/>
-      <c r="B35" s="102"/>
-      <c r="C35" s="102"/>
-      <c r="D35" s="102"/>
-      <c r="E35" s="102"/>
-      <c r="F35" s="102"/>
-      <c r="G35" s="102"/>
-      <c r="H35" s="107"/>
+      <c r="A35" s="100"/>
+      <c r="B35" s="98"/>
+      <c r="C35" s="98"/>
+      <c r="D35" s="98"/>
+      <c r="E35" s="98"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="98"/>
+      <c r="H35" s="103"/>
     </row>
     <row r="36" spans="1:8" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A36" s="108" t="s">
+      <c r="A36" s="104" t="s">
         <v>594</v>
       </c>
-      <c r="B36" s="109" t="s">
+      <c r="B36" s="105" t="s">
         <v>595</v>
       </c>
-      <c r="C36" s="109" t="s">
+      <c r="C36" s="105" t="s">
         <v>596</v>
       </c>
-      <c r="D36" s="109"/>
-      <c r="E36" s="109"/>
-      <c r="F36" s="109" t="s">
+      <c r="D36" s="105"/>
+      <c r="E36" s="105"/>
+      <c r="F36" s="105" t="s">
         <v>597</v>
       </c>
-      <c r="G36" s="109"/>
-      <c r="H36" s="110" t="s">
+      <c r="G36" s="105"/>
+      <c r="H36" s="106" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A37" s="115"/>
-      <c r="B37" s="115"/>
-      <c r="C37" s="115"/>
-      <c r="D37" s="115"/>
-      <c r="E37" s="115"/>
-      <c r="F37" s="115"/>
-      <c r="G37" s="115"/>
-      <c r="H37" s="115"/>
+      <c r="A37" s="111"/>
+      <c r="B37" s="111"/>
+      <c r="C37" s="111"/>
+      <c r="D37" s="111"/>
+      <c r="E37" s="111"/>
+      <c r="F37" s="111"/>
+      <c r="G37" s="111"/>
+      <c r="H37" s="111"/>
     </row>
     <row r="38" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A38" s="115"/>
-      <c r="B38" s="115"/>
-      <c r="C38" s="115"/>
-      <c r="D38" s="115"/>
-      <c r="E38" s="115"/>
-      <c r="F38" s="115"/>
-      <c r="G38" s="115"/>
-      <c r="H38" s="115"/>
+      <c r="A38" s="111"/>
+      <c r="B38" s="111"/>
+      <c r="C38" s="111"/>
+      <c r="D38" s="111"/>
+      <c r="E38" s="111"/>
+      <c r="F38" s="111"/>
+      <c r="G38" s="111"/>
+      <c r="H38" s="111"/>
     </row>
     <row r="39" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A39" s="115" t="s">
+      <c r="A39" s="111" t="s">
         <v>599</v>
       </c>
-      <c r="B39" s="115" t="s">
+      <c r="B39" s="111" t="s">
         <v>600</v>
       </c>
-      <c r="C39" s="101"/>
-      <c r="D39" s="115"/>
-      <c r="E39" s="115"/>
-      <c r="F39" s="115"/>
-      <c r="G39" s="115"/>
-      <c r="H39" s="115"/>
+      <c r="C39" s="97"/>
+      <c r="D39" s="111"/>
+      <c r="E39" s="111"/>
+      <c r="F39" s="111"/>
+      <c r="G39" s="111"/>
+      <c r="H39" s="111"/>
     </row>
     <row r="40" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A40" s="115"/>
-      <c r="B40" s="115" t="s">
+      <c r="A40" s="111"/>
+      <c r="B40" s="111" t="s">
         <v>601</v>
       </c>
-      <c r="C40" s="101"/>
-      <c r="D40" s="115"/>
-      <c r="E40" s="115"/>
-      <c r="F40" s="115"/>
-      <c r="G40" s="115"/>
-      <c r="H40" s="115"/>
+      <c r="C40" s="97"/>
+      <c r="D40" s="111"/>
+      <c r="E40" s="111"/>
+      <c r="F40" s="111"/>
+      <c r="G40" s="111"/>
+      <c r="H40" s="111"/>
     </row>
     <row r="41" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A41" s="115"/>
-      <c r="B41" s="115" t="s">
+      <c r="A41" s="111"/>
+      <c r="B41" s="111" t="s">
         <v>602</v>
       </c>
-      <c r="C41" s="101"/>
-      <c r="D41" s="115"/>
-      <c r="E41" s="115"/>
-      <c r="F41" s="115"/>
-      <c r="G41" s="115"/>
-      <c r="H41" s="115"/>
+      <c r="C41" s="97"/>
+      <c r="D41" s="111"/>
+      <c r="E41" s="111"/>
+      <c r="F41" s="111"/>
+      <c r="G41" s="111"/>
+      <c r="H41" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8507,10 +8640,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="27" customHeight="1">
-      <c r="A1" s="207" t="s">
+      <c r="A1" s="198" t="s">
         <v>196</v>
       </c>
-      <c r="B1" s="208"/>
+      <c r="B1" s="199"/>
     </row>
     <row r="3" spans="1:16" s="13" customFormat="1" ht="25.5">
       <c r="A3" s="32" t="s">
@@ -9034,10 +9167,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20.25">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="200" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="210"/>
+      <c r="B1" s="201"/>
     </row>
     <row r="3" spans="1:15" s="13" customFormat="1" ht="25.5">
       <c r="A3" s="32" t="s">
@@ -9449,10 +9582,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" customHeight="1">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="200" t="s">
         <v>197</v>
       </c>
-      <c r="B1" s="210"/>
+      <c r="B1" s="201"/>
     </row>
     <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5">
       <c r="A3" s="32" t="s">
@@ -9728,10 +9861,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="200" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="211"/>
+      <c r="B1" s="202"/>
     </row>
     <row r="3" spans="1:12" s="13" customFormat="1" ht="25.5">
       <c r="A3" s="32" t="s">
@@ -10228,10 +10361,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="200" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="210"/>
+      <c r="B1" s="201"/>
     </row>
     <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5">
       <c r="A3" s="32" t="s">

</xml_diff>